<commit_message>
se agregó los accesos a al super usuario o admin para el mantenimiento de empresa, sede y consultorio
</commit_message>
<xml_diff>
--- a/Requerimientos/cronograma - AMPLIACIÓN DEL SISTEMA DATA MEDIC.xlsx
+++ b/Requerimientos/cronograma - AMPLIACIÓN DEL SISTEMA DATA MEDIC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DataMedic\Requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588E10A1-1052-49F7-A14C-0D685D3674AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B4E3C2-23BB-40E9-B1F9-081F72C739E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,6 +31,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Acer</author>
+  </authors>
+  <commentList>
+    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{3F838752-99D3-4118-AA78-846F51450521}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Acer:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+se agregó más tablas a la base de datos:
+a. Hora_atencion_doctor
+b. Otra_especializacion</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
   <si>
@@ -62,13 +98,6 @@
   </si>
   <si>
     <t>Inicio</t>
-  </si>
-  <si>
-    <t>Agregar el mantenimiento completo para la: Empresa, Sede, Consultorio</t>
-  </si>
-  <si>
-    <t>Diseñar el modelo lógico y la estructura que tendrá las tablas: Empresa, Sede y Consultorio. 
-Dar acceso a los usuarios correspondiente: Super Usuario: Empresa, Gerente: Sede y Consultorio</t>
   </si>
   <si>
     <t>Agregar al usuario el consultorio al que pertenece y actualizar el mantenimiento usuario</t>
@@ -184,17 +213,33 @@
     <t>PM: 6:30 - 9:30</t>
   </si>
   <si>
+    <t xml:space="preserve">Diseñar el modelo lógico y la estructura que tendrá las tablas: Empresa, Sede y Consultorio. 
+</t>
+  </si>
+  <si>
     <t>Java Web Developer: 
-                                   a. Sesión 1
+                                   a. Sesión 1 (20%) minuto 55 del video.
                                    b. Estudiar POO teoría
-                                   c. Prácticar POO con ejercicios que yo mismo proponga</t>
+                                       - Encapsulamiento 100%
+                                   c. Prácticar POO con ejercicios que yo mismo proponga
+                                       - Encapsulamiento 100%</t>
+  </si>
+  <si>
+    <t>Agregar el mantenimiento completo para la: 
+                                     a. Empresa
+                                     b. Sede
+                                     c. Consultorio 
+                                     d. cita
+                                     e. hora_atencion_doctor
+                                     f. otra_especialización
+Dar acceso a los usuarios correspondiente: Super Usuario: Empresa, Gerente: Sede y Consultorio (100%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -445,6 +490,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="31">
@@ -974,6 +1032,24 @@
     <xf numFmtId="0" fontId="33" fillId="30" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="25" fillId="28" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="28" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="30" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="25" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -995,34 +1071,16 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="25" fillId="28" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="28" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="30" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1347,11 +1405,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1365,32 +1423,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
+      <c r="A2" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
@@ -1420,7 +1478,7 @@
         <v>5</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1428,30 +1486,30 @@
         <v>1</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="C6" s="9">
         <v>1</v>
       </c>
-      <c r="D6" s="40">
+      <c r="D6" s="33">
         <v>43990</v>
       </c>
-      <c r="E6" s="41"/>
+      <c r="E6" s="34"/>
       <c r="F6" s="12">
-        <v>0</v>
-      </c>
-      <c r="G6" s="44" t="s">
-        <v>25</v>
+        <v>1</v>
+      </c>
+      <c r="G6" s="37" t="s">
+        <v>23</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
     </row>
-    <row r="7" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="7" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>2</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C7" s="9">
         <v>2</v>
@@ -1463,28 +1521,28 @@
         <v>43992</v>
       </c>
       <c r="F7" s="12">
-        <v>0</v>
-      </c>
-      <c r="G7" s="44"/>
+        <v>0.1</v>
+      </c>
+      <c r="G7" s="37"/>
     </row>
     <row r="8" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>3</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8" s="9">
         <v>1</v>
       </c>
-      <c r="D8" s="42">
+      <c r="D8" s="35">
         <v>43993</v>
       </c>
-      <c r="E8" s="43"/>
+      <c r="E8" s="36"/>
       <c r="F8" s="12">
         <v>0</v>
       </c>
-      <c r="G8" s="44"/>
+      <c r="G8" s="37"/>
       <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1492,7 +1550,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" s="17">
         <v>2</v>
@@ -1506,14 +1564,14 @@
       <c r="F9" s="12">
         <v>0</v>
       </c>
-      <c r="G9" s="44"/>
+      <c r="G9" s="37"/>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
         <v>5</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" s="17">
         <v>1</v>
@@ -1527,7 +1585,7 @@
       <c r="F10" s="12">
         <v>0</v>
       </c>
-      <c r="G10" s="44"/>
+      <c r="G10" s="37"/>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
       <c r="J10" s="26"/>
@@ -1537,19 +1595,19 @@
         <v>6</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C11" s="9">
         <v>1</v>
       </c>
-      <c r="D11" s="38">
+      <c r="D11" s="44">
         <v>43997</v>
       </c>
-      <c r="E11" s="39"/>
+      <c r="E11" s="45"/>
       <c r="F11" s="12">
         <v>0</v>
       </c>
-      <c r="G11" s="44"/>
+      <c r="G11" s="37"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
@@ -1559,26 +1617,26 @@
         <v>7</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C12" s="9">
         <v>1</v>
       </c>
-      <c r="D12" s="38">
+      <c r="D12" s="44">
         <v>43998</v>
       </c>
-      <c r="E12" s="39"/>
+      <c r="E12" s="45"/>
       <c r="F12" s="12">
         <v>0</v>
       </c>
-      <c r="G12" s="44"/>
+      <c r="G12" s="37"/>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>8</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13" s="9">
         <v>2</v>
@@ -1592,14 +1650,14 @@
       <c r="F13" s="12">
         <v>0</v>
       </c>
-      <c r="G13" s="44"/>
+      <c r="G13" s="37"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>9</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1">
         <v>2</v>
@@ -1613,63 +1671,63 @@
       <c r="F14" s="12">
         <v>0</v>
       </c>
-      <c r="G14" s="44"/>
+      <c r="G14" s="37"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>10</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C15" s="9">
         <v>1</v>
       </c>
-      <c r="D15" s="42">
+      <c r="D15" s="35">
         <v>44004</v>
       </c>
-      <c r="E15" s="43"/>
+      <c r="E15" s="36"/>
       <c r="F15" s="12">
         <v>0</v>
       </c>
-      <c r="G15" s="44"/>
+      <c r="G15" s="37"/>
     </row>
     <row r="16" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>11</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C16" s="9">
         <v>1</v>
       </c>
-      <c r="D16" s="42">
+      <c r="D16" s="35">
         <v>44005</v>
       </c>
-      <c r="E16" s="43"/>
+      <c r="E16" s="36"/>
       <c r="F16" s="12">
         <v>0</v>
       </c>
-      <c r="G16" s="44"/>
+      <c r="G16" s="37"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>12</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C17" s="13"/>
-      <c r="D17" s="33">
+      <c r="D17" s="39">
         <v>44006</v>
       </c>
-      <c r="E17" s="34"/>
+      <c r="E17" s="40"/>
       <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C18" s="22">
         <f>SUM(C6:C16)</f>
@@ -1678,39 +1736,39 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="35" t="s">
+      <c r="D20" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="35"/>
-      <c r="F20" s="37">
-        <f>SUM(F6:F16)/10</f>
-        <v>0</v>
+      <c r="E20" s="41"/>
+      <c r="F20" s="43">
+        <f>SUM(F6:F16)/11</f>
+        <v>0.1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="10"/>
-      <c r="C21" s="36"/>
+      <c r="C21" s="42"/>
       <c r="D21" s="18" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="37"/>
+      <c r="F21" s="43"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
-      <c r="C22" s="36"/>
+      <c r="C22" s="42"/>
       <c r="D22" s="4">
         <v>43990</v>
       </c>
       <c r="E22" s="4">
         <v>44006</v>
       </c>
-      <c r="F22" s="37"/>
+      <c r="F22" s="43"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
@@ -1720,6 +1778,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="G6:G16"/>
@@ -1728,15 +1792,10 @@
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1744,8 +1803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{408A92BF-85F0-40E9-8A2F-FC2971961963}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1760,32 +1819,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
+      <c r="A2" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -1807,30 +1866,30 @@
         <v>5</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>1</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="47">
+        <v>39</v>
+      </c>
+      <c r="C6" s="46">
         <v>5</v>
       </c>
-      <c r="D6" s="46">
+      <c r="D6" s="48">
         <v>43990</v>
       </c>
-      <c r="E6" s="46">
+      <c r="E6" s="48">
         <v>43994</v>
       </c>
       <c r="F6" s="12">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="G6" s="32" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1838,16 +1897,16 @@
         <v>2</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
+        <v>27</v>
+      </c>
+      <c r="C7" s="49"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
       <c r="F7" s="12">
         <v>0</v>
       </c>
       <c r="G7" s="32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1855,20 +1914,20 @@
         <v>3</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="48"/>
-      <c r="D8" s="46">
+        <v>26</v>
+      </c>
+      <c r="C8" s="49"/>
+      <c r="D8" s="48">
         <v>43997</v>
       </c>
-      <c r="E8" s="46">
+      <c r="E8" s="48">
         <v>44001</v>
       </c>
       <c r="F8" s="12">
         <v>0</v>
       </c>
       <c r="G8" s="32" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H8" s="27"/>
     </row>
@@ -1877,16 +1936,16 @@
         <v>4</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
+        <v>28</v>
+      </c>
+      <c r="C9" s="49"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
       <c r="F9" s="12">
         <v>0</v>
       </c>
       <c r="G9" s="32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1894,20 +1953,20 @@
         <v>5</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="48"/>
-      <c r="D10" s="46">
+        <v>29</v>
+      </c>
+      <c r="C10" s="49"/>
+      <c r="D10" s="48">
         <v>44004</v>
       </c>
-      <c r="E10" s="46">
+      <c r="E10" s="48">
         <v>44008</v>
       </c>
       <c r="F10" s="12">
         <v>0</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1915,16 +1974,16 @@
         <v>6</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="48"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
+        <v>30</v>
+      </c>
+      <c r="C11" s="49"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
       <c r="F11" s="12">
         <v>0</v>
       </c>
       <c r="G11" s="32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H11" s="29"/>
       <c r="I11" s="29"/>
@@ -1935,20 +1994,20 @@
         <v>7</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="46">
+        <v>31</v>
+      </c>
+      <c r="C12" s="49"/>
+      <c r="D12" s="48">
         <v>44004</v>
       </c>
-      <c r="E12" s="46">
+      <c r="E12" s="48">
         <v>44008</v>
       </c>
       <c r="F12" s="12">
         <v>0</v>
       </c>
       <c r="G12" s="32" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1956,16 +2015,16 @@
         <v>8</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
+        <v>32</v>
+      </c>
+      <c r="C13" s="47"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
       <c r="F13" s="12">
         <v>0</v>
       </c>
       <c r="G13" s="32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1973,22 +2032,22 @@
         <v>9</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="47">
+        <v>33</v>
+      </c>
+      <c r="C14" s="46">
         <v>6</v>
       </c>
-      <c r="D14" s="46">
+      <c r="D14" s="48">
         <v>44011</v>
       </c>
-      <c r="E14" s="46">
+      <c r="E14" s="48">
         <v>44016</v>
       </c>
       <c r="F14" s="12">
         <v>0</v>
       </c>
       <c r="G14" s="32" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -1996,16 +2055,16 @@
         <v>10</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="49"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
+        <v>34</v>
+      </c>
+      <c r="C15" s="47"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
       <c r="F15" s="12">
         <v>0</v>
       </c>
       <c r="G15" s="32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2013,9 +2072,9 @@
         <v>9</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="47">
+        <v>35</v>
+      </c>
+      <c r="C16" s="46">
         <v>5</v>
       </c>
       <c r="D16" s="28">
@@ -2028,7 +2087,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -2036,9 +2095,9 @@
         <v>9</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="49"/>
+        <v>36</v>
+      </c>
+      <c r="C17" s="47"/>
       <c r="D17" s="28">
         <v>44025</v>
       </c>
@@ -2049,12 +2108,12 @@
         <v>0</v>
       </c>
       <c r="G17" s="32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="30" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C18" s="22">
         <v>31</v>
@@ -2062,39 +2121,39 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="29"/>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="36" t="s">
+      <c r="D20" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="36"/>
-      <c r="F20" s="37">
+      <c r="E20" s="42"/>
+      <c r="F20" s="43">
         <f>SUM(F6:F17)/12</f>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="29"/>
-      <c r="C21" s="36"/>
+      <c r="C21" s="42"/>
       <c r="D21" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="37"/>
+      <c r="F21" s="43"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
-      <c r="C22" s="36"/>
+      <c r="C22" s="42"/>
       <c r="D22" s="4">
         <v>43990</v>
       </c>
       <c r="E22" s="28">
         <v>44029</v>
       </c>
-      <c r="F22" s="37"/>
+      <c r="F22" s="43"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="29"/>
@@ -2104,11 +2163,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="D14:D15"/>
@@ -2123,6 +2177,11 @@
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
   </mergeCells>
   <phoneticPr fontId="31" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
se terminó el mantenimiento de empresa
</commit_message>
<xml_diff>
--- a/Requerimientos/cronograma - AMPLIACIÓN DEL SISTEMA DATA MEDIC.xlsx
+++ b/Requerimientos/cronograma - AMPLIACIÓN DEL SISTEMA DATA MEDIC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DataMedic\Requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B4E3C2-23BB-40E9-B1F9-081F72C739E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B575E43B-825B-4579-8BFD-61BDEA6FB247}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -226,12 +226,13 @@
   </si>
   <si>
     <t>Agregar el mantenimiento completo para la: 
-                                     a. Empresa
+                                     a. Empresa ( al 100%)
                                      b. Sede
                                      c. Consultorio 
-                                     d. cita
-                                     e. hora_atencion_doctor
-                                     f. otra_especialización
+                                     d. Área
+                                     e. cita
+                                     f. hora_atencion_doctor
+                                     g. otra_especialización
 Dar acceso a los usuarios correspondiente: Super Usuario: Empresa, Gerente: Sede y Consultorio (100%)</t>
   </si>
 </sst>
@@ -1032,6 +1033,27 @@
     <xf numFmtId="0" fontId="33" fillId="30" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="25" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="26" fillId="27" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="25" fillId="28" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1050,37 +1072,16 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="25" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="26" fillId="27" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1409,7 +1410,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1423,32 +1424,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
+      <c r="A3" s="45"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
@@ -1491,20 +1492,20 @@
       <c r="C6" s="9">
         <v>1</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="40">
         <v>43990</v>
       </c>
-      <c r="E6" s="34"/>
+      <c r="E6" s="41"/>
       <c r="F6" s="12">
         <v>1</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="G6" s="44" t="s">
         <v>23</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
     </row>
-    <row r="7" spans="1:10" s="7" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="7" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>2</v>
       </c>
@@ -1521,9 +1522,9 @@
         <v>43992</v>
       </c>
       <c r="F7" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="G7" s="37"/>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G7" s="44"/>
     </row>
     <row r="8" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
@@ -1535,14 +1536,14 @@
       <c r="C8" s="9">
         <v>1</v>
       </c>
-      <c r="D8" s="35">
+      <c r="D8" s="42">
         <v>43993</v>
       </c>
-      <c r="E8" s="36"/>
+      <c r="E8" s="43"/>
       <c r="F8" s="12">
         <v>0</v>
       </c>
-      <c r="G8" s="37"/>
+      <c r="G8" s="44"/>
       <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1564,7 +1565,7 @@
       <c r="F9" s="12">
         <v>0</v>
       </c>
-      <c r="G9" s="37"/>
+      <c r="G9" s="44"/>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
@@ -1585,7 +1586,7 @@
       <c r="F10" s="12">
         <v>0</v>
       </c>
-      <c r="G10" s="37"/>
+      <c r="G10" s="44"/>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
       <c r="J10" s="26"/>
@@ -1600,14 +1601,14 @@
       <c r="C11" s="9">
         <v>1</v>
       </c>
-      <c r="D11" s="44">
+      <c r="D11" s="38">
         <v>43997</v>
       </c>
-      <c r="E11" s="45"/>
+      <c r="E11" s="39"/>
       <c r="F11" s="12">
         <v>0</v>
       </c>
-      <c r="G11" s="37"/>
+      <c r="G11" s="44"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
@@ -1622,14 +1623,14 @@
       <c r="C12" s="9">
         <v>1</v>
       </c>
-      <c r="D12" s="44">
+      <c r="D12" s="38">
         <v>43998</v>
       </c>
-      <c r="E12" s="45"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="12">
         <v>0</v>
       </c>
-      <c r="G12" s="37"/>
+      <c r="G12" s="44"/>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
@@ -1650,7 +1651,7 @@
       <c r="F13" s="12">
         <v>0</v>
       </c>
-      <c r="G13" s="37"/>
+      <c r="G13" s="44"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -1671,7 +1672,7 @@
       <c r="F14" s="12">
         <v>0</v>
       </c>
-      <c r="G14" s="37"/>
+      <c r="G14" s="44"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
@@ -1683,14 +1684,14 @@
       <c r="C15" s="9">
         <v>1</v>
       </c>
-      <c r="D15" s="35">
+      <c r="D15" s="42">
         <v>44004</v>
       </c>
-      <c r="E15" s="36"/>
+      <c r="E15" s="43"/>
       <c r="F15" s="12">
         <v>0</v>
       </c>
-      <c r="G15" s="37"/>
+      <c r="G15" s="44"/>
     </row>
     <row r="16" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
@@ -1702,14 +1703,14 @@
       <c r="C16" s="9">
         <v>1</v>
       </c>
-      <c r="D16" s="35">
+      <c r="D16" s="42">
         <v>44005</v>
       </c>
-      <c r="E16" s="36"/>
+      <c r="E16" s="43"/>
       <c r="F16" s="12">
         <v>0</v>
       </c>
-      <c r="G16" s="37"/>
+      <c r="G16" s="44"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
@@ -1719,10 +1720,10 @@
         <v>16</v>
       </c>
       <c r="C17" s="13"/>
-      <c r="D17" s="39">
+      <c r="D17" s="33">
         <v>44006</v>
       </c>
-      <c r="E17" s="40"/>
+      <c r="E17" s="34"/>
       <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1736,39 +1737,39 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="41" t="s">
+      <c r="D20" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="41"/>
-      <c r="F20" s="43">
+      <c r="E20" s="35"/>
+      <c r="F20" s="37">
         <f>SUM(F6:F16)/11</f>
-        <v>0.1</v>
+        <v>0.11636363636363636</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="10"/>
-      <c r="C21" s="42"/>
+      <c r="C21" s="36"/>
       <c r="D21" s="18" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="43"/>
+      <c r="F21" s="37"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
-      <c r="C22" s="42"/>
+      <c r="C22" s="36"/>
       <c r="D22" s="4">
         <v>43990</v>
       </c>
       <c r="E22" s="4">
         <v>44006</v>
       </c>
-      <c r="F22" s="43"/>
+      <c r="F22" s="37"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
@@ -1778,12 +1779,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="G6:G16"/>
@@ -1792,6 +1787,12 @@
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1819,32 +1820,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
+      <c r="A3" s="45"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -1876,13 +1877,13 @@
       <c r="B6" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="46">
+      <c r="C6" s="47">
         <v>5</v>
       </c>
-      <c r="D6" s="48">
+      <c r="D6" s="46">
         <v>43990</v>
       </c>
-      <c r="E6" s="48">
+      <c r="E6" s="46">
         <v>43994</v>
       </c>
       <c r="F6" s="12">
@@ -1899,9 +1900,9 @@
       <c r="B7" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
       <c r="F7" s="12">
         <v>0</v>
       </c>
@@ -1916,11 +1917,11 @@
       <c r="B8" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="48">
+      <c r="C8" s="48"/>
+      <c r="D8" s="46">
         <v>43997</v>
       </c>
-      <c r="E8" s="48">
+      <c r="E8" s="46">
         <v>44001</v>
       </c>
       <c r="F8" s="12">
@@ -1938,9 +1939,9 @@
       <c r="B9" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
       <c r="F9" s="12">
         <v>0</v>
       </c>
@@ -1955,11 +1956,11 @@
       <c r="B10" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="48">
+      <c r="C10" s="48"/>
+      <c r="D10" s="46">
         <v>44004</v>
       </c>
-      <c r="E10" s="48">
+      <c r="E10" s="46">
         <v>44008</v>
       </c>
       <c r="F10" s="12">
@@ -1976,9 +1977,9 @@
       <c r="B11" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
       <c r="F11" s="12">
         <v>0</v>
       </c>
@@ -1996,11 +1997,11 @@
       <c r="B12" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="48">
+      <c r="C12" s="48"/>
+      <c r="D12" s="46">
         <v>44004</v>
       </c>
-      <c r="E12" s="48">
+      <c r="E12" s="46">
         <v>44008</v>
       </c>
       <c r="F12" s="12">
@@ -2017,9 +2018,9 @@
       <c r="B13" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="47"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
       <c r="F13" s="12">
         <v>0</v>
       </c>
@@ -2034,13 +2035,13 @@
       <c r="B14" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="46">
+      <c r="C14" s="47">
         <v>6</v>
       </c>
-      <c r="D14" s="48">
+      <c r="D14" s="46">
         <v>44011</v>
       </c>
-      <c r="E14" s="48">
+      <c r="E14" s="46">
         <v>44016</v>
       </c>
       <c r="F14" s="12">
@@ -2057,9 +2058,9 @@
       <c r="B15" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
       <c r="F15" s="12">
         <v>0</v>
       </c>
@@ -2074,7 +2075,7 @@
       <c r="B16" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="46">
+      <c r="C16" s="47">
         <v>5</v>
       </c>
       <c r="D16" s="28">
@@ -2097,7 +2098,7 @@
       <c r="B17" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="47"/>
+      <c r="C17" s="49"/>
       <c r="D17" s="28">
         <v>44025</v>
       </c>
@@ -2121,39 +2122,39 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="29"/>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="D20" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="42"/>
-      <c r="F20" s="43">
+      <c r="E20" s="36"/>
+      <c r="F20" s="37">
         <f>SUM(F6:F17)/12</f>
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="29"/>
-      <c r="C21" s="42"/>
+      <c r="C21" s="36"/>
       <c r="D21" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="43"/>
+      <c r="F21" s="37"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
-      <c r="C22" s="42"/>
+      <c r="C22" s="36"/>
       <c r="D22" s="4">
         <v>43990</v>
       </c>
       <c r="E22" s="28">
         <v>44029</v>
       </c>
-      <c r="F22" s="43"/>
+      <c r="F22" s="37"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="29"/>
@@ -2163,6 +2164,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="D14:D15"/>
@@ -2177,11 +2183,6 @@
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
   </mergeCells>
   <phoneticPr fontId="31" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
se agregó el mantenimiento completo de la sede
</commit_message>
<xml_diff>
--- a/Requerimientos/cronograma - AMPLIACIÓN DEL SISTEMA DATA MEDIC.xlsx
+++ b/Requerimientos/cronograma - AMPLIACIÓN DEL SISTEMA DATA MEDIC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DataMedic\Requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B575E43B-825B-4579-8BFD-61BDEA6FB247}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A408342A-B0E0-4DF6-8470-F60486A39EEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1033,6 +1033,24 @@
     <xf numFmtId="0" fontId="33" fillId="30" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="25" fillId="28" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="28" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="30" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="25" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1054,34 +1072,16 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="25" fillId="28" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="28" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="30" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1410,7 +1410,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1424,32 +1424,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
@@ -1492,14 +1492,14 @@
       <c r="C6" s="9">
         <v>1</v>
       </c>
-      <c r="D6" s="40">
+      <c r="D6" s="33">
         <v>43990</v>
       </c>
-      <c r="E6" s="41"/>
+      <c r="E6" s="34"/>
       <c r="F6" s="12">
         <v>1</v>
       </c>
-      <c r="G6" s="44" t="s">
+      <c r="G6" s="37" t="s">
         <v>23</v>
       </c>
       <c r="H6" s="26"/>
@@ -1524,7 +1524,7 @@
       <c r="F7" s="12">
         <v>0.28000000000000003</v>
       </c>
-      <c r="G7" s="44"/>
+      <c r="G7" s="37"/>
     </row>
     <row r="8" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
@@ -1536,14 +1536,14 @@
       <c r="C8" s="9">
         <v>1</v>
       </c>
-      <c r="D8" s="42">
+      <c r="D8" s="35">
         <v>43993</v>
       </c>
-      <c r="E8" s="43"/>
+      <c r="E8" s="36"/>
       <c r="F8" s="12">
         <v>0</v>
       </c>
-      <c r="G8" s="44"/>
+      <c r="G8" s="37"/>
       <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1565,7 +1565,7 @@
       <c r="F9" s="12">
         <v>0</v>
       </c>
-      <c r="G9" s="44"/>
+      <c r="G9" s="37"/>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
@@ -1586,7 +1586,7 @@
       <c r="F10" s="12">
         <v>0</v>
       </c>
-      <c r="G10" s="44"/>
+      <c r="G10" s="37"/>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
       <c r="J10" s="26"/>
@@ -1601,14 +1601,14 @@
       <c r="C11" s="9">
         <v>1</v>
       </c>
-      <c r="D11" s="38">
+      <c r="D11" s="44">
         <v>43997</v>
       </c>
-      <c r="E11" s="39"/>
+      <c r="E11" s="45"/>
       <c r="F11" s="12">
         <v>0</v>
       </c>
-      <c r="G11" s="44"/>
+      <c r="G11" s="37"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
@@ -1623,14 +1623,14 @@
       <c r="C12" s="9">
         <v>1</v>
       </c>
-      <c r="D12" s="38">
+      <c r="D12" s="44">
         <v>43998</v>
       </c>
-      <c r="E12" s="39"/>
+      <c r="E12" s="45"/>
       <c r="F12" s="12">
         <v>0</v>
       </c>
-      <c r="G12" s="44"/>
+      <c r="G12" s="37"/>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
@@ -1651,7 +1651,7 @@
       <c r="F13" s="12">
         <v>0</v>
       </c>
-      <c r="G13" s="44"/>
+      <c r="G13" s="37"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -1672,7 +1672,7 @@
       <c r="F14" s="12">
         <v>0</v>
       </c>
-      <c r="G14" s="44"/>
+      <c r="G14" s="37"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
@@ -1684,14 +1684,14 @@
       <c r="C15" s="9">
         <v>1</v>
       </c>
-      <c r="D15" s="42">
+      <c r="D15" s="35">
         <v>44004</v>
       </c>
-      <c r="E15" s="43"/>
+      <c r="E15" s="36"/>
       <c r="F15" s="12">
         <v>0</v>
       </c>
-      <c r="G15" s="44"/>
+      <c r="G15" s="37"/>
     </row>
     <row r="16" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
@@ -1703,14 +1703,14 @@
       <c r="C16" s="9">
         <v>1</v>
       </c>
-      <c r="D16" s="42">
+      <c r="D16" s="35">
         <v>44005</v>
       </c>
-      <c r="E16" s="43"/>
+      <c r="E16" s="36"/>
       <c r="F16" s="12">
         <v>0</v>
       </c>
-      <c r="G16" s="44"/>
+      <c r="G16" s="37"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
@@ -1720,10 +1720,10 @@
         <v>16</v>
       </c>
       <c r="C17" s="13"/>
-      <c r="D17" s="33">
+      <c r="D17" s="39">
         <v>44006</v>
       </c>
-      <c r="E17" s="34"/>
+      <c r="E17" s="40"/>
       <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1737,39 +1737,39 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="35" t="s">
+      <c r="D20" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="35"/>
-      <c r="F20" s="37">
+      <c r="E20" s="41"/>
+      <c r="F20" s="43">
         <f>SUM(F6:F16)/11</f>
         <v>0.11636363636363636</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="10"/>
-      <c r="C21" s="36"/>
+      <c r="C21" s="42"/>
       <c r="D21" s="18" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="37"/>
+      <c r="F21" s="43"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
-      <c r="C22" s="36"/>
+      <c r="C22" s="42"/>
       <c r="D22" s="4">
         <v>43990</v>
       </c>
       <c r="E22" s="4">
         <v>44006</v>
       </c>
-      <c r="F22" s="37"/>
+      <c r="F22" s="43"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
@@ -1779,6 +1779,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="G6:G16"/>
@@ -1787,12 +1793,6 @@
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1820,32 +1820,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -1877,13 +1877,13 @@
       <c r="B6" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="47">
+      <c r="C6" s="46">
         <v>5</v>
       </c>
-      <c r="D6" s="46">
+      <c r="D6" s="48">
         <v>43990</v>
       </c>
-      <c r="E6" s="46">
+      <c r="E6" s="48">
         <v>43994</v>
       </c>
       <c r="F6" s="12">
@@ -1900,9 +1900,9 @@
       <c r="B7" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
       <c r="F7" s="12">
         <v>0</v>
       </c>
@@ -1917,11 +1917,11 @@
       <c r="B8" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="48"/>
-      <c r="D8" s="46">
+      <c r="C8" s="49"/>
+      <c r="D8" s="48">
         <v>43997</v>
       </c>
-      <c r="E8" s="46">
+      <c r="E8" s="48">
         <v>44001</v>
       </c>
       <c r="F8" s="12">
@@ -1939,9 +1939,9 @@
       <c r="B9" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
       <c r="F9" s="12">
         <v>0</v>
       </c>
@@ -1956,11 +1956,11 @@
       <c r="B10" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="48"/>
-      <c r="D10" s="46">
+      <c r="C10" s="49"/>
+      <c r="D10" s="48">
         <v>44004</v>
       </c>
-      <c r="E10" s="46">
+      <c r="E10" s="48">
         <v>44008</v>
       </c>
       <c r="F10" s="12">
@@ -1977,9 +1977,9 @@
       <c r="B11" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="48"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
       <c r="F11" s="12">
         <v>0</v>
       </c>
@@ -1997,11 +1997,11 @@
       <c r="B12" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="46">
+      <c r="C12" s="49"/>
+      <c r="D12" s="48">
         <v>44004</v>
       </c>
-      <c r="E12" s="46">
+      <c r="E12" s="48">
         <v>44008</v>
       </c>
       <c r="F12" s="12">
@@ -2018,9 +2018,9 @@
       <c r="B13" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
       <c r="F13" s="12">
         <v>0</v>
       </c>
@@ -2035,13 +2035,13 @@
       <c r="B14" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="47">
+      <c r="C14" s="46">
         <v>6</v>
       </c>
-      <c r="D14" s="46">
+      <c r="D14" s="48">
         <v>44011</v>
       </c>
-      <c r="E14" s="46">
+      <c r="E14" s="48">
         <v>44016</v>
       </c>
       <c r="F14" s="12">
@@ -2058,9 +2058,9 @@
       <c r="B15" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="49"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
       <c r="F15" s="12">
         <v>0</v>
       </c>
@@ -2075,7 +2075,7 @@
       <c r="B16" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="47">
+      <c r="C16" s="46">
         <v>5</v>
       </c>
       <c r="D16" s="28">
@@ -2098,7 +2098,7 @@
       <c r="B17" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="49"/>
+      <c r="C17" s="47"/>
       <c r="D17" s="28">
         <v>44025</v>
       </c>
@@ -2122,39 +2122,39 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="29"/>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="36" t="s">
+      <c r="D20" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="36"/>
-      <c r="F20" s="37">
+      <c r="E20" s="42"/>
+      <c r="F20" s="43">
         <f>SUM(F6:F17)/12</f>
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="29"/>
-      <c r="C21" s="36"/>
+      <c r="C21" s="42"/>
       <c r="D21" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="37"/>
+      <c r="F21" s="43"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
-      <c r="C22" s="36"/>
+      <c r="C22" s="42"/>
       <c r="D22" s="4">
         <v>43990</v>
       </c>
       <c r="E22" s="28">
         <v>44029</v>
       </c>
-      <c r="F22" s="37"/>
+      <c r="F22" s="43"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="29"/>
@@ -2164,11 +2164,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="D14:D15"/>
@@ -2183,6 +2178,11 @@
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
   </mergeCells>
   <phoneticPr fontId="31" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
se agregó el listar y se arregló el formulario del consultorio
</commit_message>
<xml_diff>
--- a/Requerimientos/cronograma - AMPLIACIÓN DEL SISTEMA DATA MEDIC.xlsx
+++ b/Requerimientos/cronograma - AMPLIACIÓN DEL SISTEMA DATA MEDIC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DataMedic\Requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A408342A-B0E0-4DF6-8470-F60486A39EEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86447455-3499-4E64-85A5-A9B4871D95A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -221,15 +221,18 @@
                                    a. Sesión 1 (20%) minuto 55 del video.
                                    b. Estudiar POO teoría
                                        - Encapsulamiento 100%
+                                       - Herencia 100%
+                                       - Polimorfismo 100%
+                                       - Interfaz 100%
                                    c. Prácticar POO con ejercicios que yo mismo proponga
                                        - Encapsulamiento 100%</t>
   </si>
   <si>
     <t>Agregar el mantenimiento completo para la: 
                                      a. Empresa ( al 100%)
-                                     b. Sede
-                                     c. Consultorio 
-                                     d. Área
+                                     b. Sede ( al 100%)
+                                     c. Consultorio
+                                     d. Área ( al 100%)
                                      e. cita
                                      f. hora_atencion_doctor
                                      g. otra_especialización
@@ -1410,7 +1413,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1522,7 +1525,7 @@
         <v>43992</v>
       </c>
       <c r="F7" s="12">
-        <v>0.28000000000000003</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="G7" s="37"/>
     </row>
@@ -1746,7 +1749,7 @@
       <c r="E20" s="41"/>
       <c r="F20" s="43">
         <f>SUM(F6:F16)/11</f>
-        <v>0.11636363636363636</v>
+        <v>0.14181818181818182</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1805,7 +1808,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20:F22"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1870,7 +1873,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>1</v>
       </c>
@@ -1887,7 +1890,7 @@
         <v>43994</v>
       </c>
       <c r="F6" s="12">
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
       <c r="G6" s="32" t="s">
         <v>24</v>
@@ -2131,7 +2134,7 @@
       <c r="E20" s="42"/>
       <c r="F20" s="43">
         <f>SUM(F6:F17)/12</f>
-        <v>2.0833333333333332E-2</v>
+        <v>3.3333333333333333E-2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
se agregó el formulario de horario atención, se implementó la funciones eliminar y leer datos. Se actualizó los campos de la tabla horario_atención
</commit_message>
<xml_diff>
--- a/Requerimientos/cronograma - AMPLIACIÓN DEL SISTEMA DATA MEDIC.xlsx
+++ b/Requerimientos/cronograma - AMPLIACIÓN DEL SISTEMA DATA MEDIC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DataMedic\Requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54CE97E0-61FD-4B5B-8ED9-D2CE54845252}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93367365-B744-4BA7-B9E7-428E2C4558A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,6 +63,32 @@
         </r>
       </text>
     </comment>
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{FFC90869-2484-4C70-A4C8-767DCAAE7BE9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Acer:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+El usuario no pertenece a ningún consultorio.
+El paciente es el que pertenece a un consultorio cuando realiza una cita
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -100,13 +126,7 @@
     <t>Inicio</t>
   </si>
   <si>
-    <t>Agregar al usuario el consultorio al que pertenece y actualizar el mantenimiento usuario</t>
-  </si>
-  <si>
     <t>Mostrar dentro del sistema, como página principal al: Gerente: Dashboard, Doctor: Citas confirmadas, Cliente: registrar sus citas y super usuario: logs.</t>
-  </si>
-  <si>
-    <t>Revisar el código que tiene la plantilla para los gráficos estadísticos y diseñar la página del dassboard</t>
   </si>
   <si>
     <t xml:space="preserve">Actualizar e implementar los nuevos logs que requiere el sistema. </t>
@@ -228,24 +248,41 @@
                                        - Encapsulamiento 100%</t>
   </si>
   <si>
+    <r>
+      <t>Agregar al usuario el consultorio al que pertenece y actualizar el mantenimiento usuario</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(LEER COMENTARIO)</t>
+    </r>
+  </si>
+  <si>
     <t>Agregar el mantenimiento completo para la: 
                                      a. Empresa ( al 100%)
                                      b. Sede ( al 100%)
                                      c. Consultorio ( al 100%)
-                                     d. Área ( al 100%)
-                                     e. Día_semana(12/06/2020)                                     
-                                     f. Horario de trabajo(12/06/2020)
-                                     g. cita(13/06/2020)
-                                     h. hora_atencion_doctor(13/06/2020)
-                                     i. otra_especialización(13/06/2020)
+                                     d. Área ( al 100%)                          
+                                     e. Horario de trabajo(al 50%)
+                                     f. cita(13/06/2020)
+                                     g. otra_especialización(13/06/2020)
 Dar acceso a los usuarios correspondiente: Super Usuario: Empresa, Gerente: Sede y Consultorio (100%)</t>
+  </si>
+  <si>
+    <t>Revisar el código que tiene la plantilla para los gráficos estadísticos y diseñar la página del dashboard</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="37" x14ac:knownFonts="1">
+  <fonts count="38" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -509,6 +546,14 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="31">
@@ -1038,6 +1083,24 @@
     <xf numFmtId="0" fontId="33" fillId="30" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="25" fillId="28" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="28" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="30" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="25" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1059,34 +1122,16 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="25" fillId="28" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="28" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="30" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1414,8 +1459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1429,32 +1474,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
+      <c r="A2" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
@@ -1484,7 +1529,7 @@
         <v>5</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1492,30 +1537,30 @@
         <v>1</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C6" s="9">
         <v>1</v>
       </c>
-      <c r="D6" s="40">
+      <c r="D6" s="33">
         <v>43990</v>
       </c>
-      <c r="E6" s="41"/>
+      <c r="E6" s="34"/>
       <c r="F6" s="12">
         <v>1</v>
       </c>
-      <c r="G6" s="44" t="s">
-        <v>23</v>
+      <c r="G6" s="37" t="s">
+        <v>21</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
     </row>
-    <row r="7" spans="1:10" s="7" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="7" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>2</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="9">
         <v>2</v>
@@ -1527,28 +1572,28 @@
         <v>43992</v>
       </c>
       <c r="F7" s="12">
-        <v>0.44</v>
-      </c>
-      <c r="G7" s="44"/>
-    </row>
-    <row r="8" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0.6</v>
+      </c>
+      <c r="G7" s="37"/>
+    </row>
+    <row r="8" spans="1:10" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>3</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="C8" s="9">
         <v>1</v>
       </c>
-      <c r="D8" s="42">
+      <c r="D8" s="35">
         <v>43993</v>
       </c>
-      <c r="E8" s="43"/>
+      <c r="E8" s="36"/>
       <c r="F8" s="12">
-        <v>0</v>
-      </c>
-      <c r="G8" s="44"/>
+        <v>1</v>
+      </c>
+      <c r="G8" s="37"/>
       <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1556,7 +1601,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9" s="17">
         <v>2</v>
@@ -1570,14 +1615,14 @@
       <c r="F9" s="12">
         <v>0</v>
       </c>
-      <c r="G9" s="44"/>
+      <c r="G9" s="37"/>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
         <v>5</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" s="17">
         <v>1</v>
@@ -1591,7 +1636,7 @@
       <c r="F10" s="12">
         <v>0</v>
       </c>
-      <c r="G10" s="44"/>
+      <c r="G10" s="37"/>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
       <c r="J10" s="26"/>
@@ -1601,19 +1646,19 @@
         <v>6</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="9">
         <v>1</v>
       </c>
-      <c r="D11" s="38">
+      <c r="D11" s="44">
         <v>43997</v>
       </c>
-      <c r="E11" s="39"/>
+      <c r="E11" s="45"/>
       <c r="F11" s="12">
         <v>0</v>
       </c>
-      <c r="G11" s="44"/>
+      <c r="G11" s="37"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
@@ -1623,26 +1668,26 @@
         <v>7</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="C12" s="9">
         <v>1</v>
       </c>
-      <c r="D12" s="38">
+      <c r="D12" s="44">
         <v>43998</v>
       </c>
-      <c r="E12" s="39"/>
+      <c r="E12" s="45"/>
       <c r="F12" s="12">
         <v>0</v>
       </c>
-      <c r="G12" s="44"/>
+      <c r="G12" s="37"/>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>8</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C13" s="9">
         <v>2</v>
@@ -1656,14 +1701,14 @@
       <c r="F13" s="12">
         <v>0</v>
       </c>
-      <c r="G13" s="44"/>
+      <c r="G13" s="37"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>9</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1">
         <v>2</v>
@@ -1677,63 +1722,63 @@
       <c r="F14" s="12">
         <v>0</v>
       </c>
-      <c r="G14" s="44"/>
+      <c r="G14" s="37"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>10</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C15" s="9">
         <v>1</v>
       </c>
-      <c r="D15" s="42">
+      <c r="D15" s="35">
         <v>44004</v>
       </c>
-      <c r="E15" s="43"/>
+      <c r="E15" s="36"/>
       <c r="F15" s="12">
         <v>0</v>
       </c>
-      <c r="G15" s="44"/>
+      <c r="G15" s="37"/>
     </row>
     <row r="16" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>11</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C16" s="9">
         <v>1</v>
       </c>
-      <c r="D16" s="42">
+      <c r="D16" s="35">
         <v>44005</v>
       </c>
-      <c r="E16" s="43"/>
+      <c r="E16" s="36"/>
       <c r="F16" s="12">
         <v>0</v>
       </c>
-      <c r="G16" s="44"/>
+      <c r="G16" s="37"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>12</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C17" s="13"/>
-      <c r="D17" s="33">
+      <c r="D17" s="39">
         <v>44006</v>
       </c>
-      <c r="E17" s="34"/>
+      <c r="E17" s="40"/>
       <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C18" s="22">
         <f>SUM(C6:C16)</f>
@@ -1742,39 +1787,39 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="35" t="s">
+      <c r="D20" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="35"/>
-      <c r="F20" s="37">
+      <c r="E20" s="41"/>
+      <c r="F20" s="43">
         <f>SUM(F6:F16)/11</f>
-        <v>0.13090909090909089</v>
+        <v>0.23636363636363636</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="10"/>
-      <c r="C21" s="36"/>
+      <c r="C21" s="42"/>
       <c r="D21" s="18" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="37"/>
+      <c r="F21" s="43"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
-      <c r="C22" s="36"/>
+      <c r="C22" s="42"/>
       <c r="D22" s="4">
         <v>43990</v>
       </c>
       <c r="E22" s="4">
         <v>44006</v>
       </c>
-      <c r="F22" s="37"/>
+      <c r="F22" s="43"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
@@ -1784,6 +1829,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="G6:G16"/>
@@ -1792,12 +1843,6 @@
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1825,32 +1870,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
+      <c r="A2" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -1872,7 +1917,7 @@
         <v>5</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -1880,22 +1925,22 @@
         <v>1</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="47">
+        <v>37</v>
+      </c>
+      <c r="C6" s="46">
         <v>5</v>
       </c>
-      <c r="D6" s="46">
+      <c r="D6" s="48">
         <v>43990</v>
       </c>
-      <c r="E6" s="46">
+      <c r="E6" s="48">
         <v>43994</v>
       </c>
       <c r="F6" s="12">
         <v>0.4</v>
       </c>
       <c r="G6" s="32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1903,16 +1948,16 @@
         <v>2</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
+        <v>25</v>
+      </c>
+      <c r="C7" s="49"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
       <c r="F7" s="12">
         <v>0</v>
       </c>
       <c r="G7" s="32" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1920,20 +1965,20 @@
         <v>3</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="48"/>
-      <c r="D8" s="46">
+        <v>24</v>
+      </c>
+      <c r="C8" s="49"/>
+      <c r="D8" s="48">
         <v>43997</v>
       </c>
-      <c r="E8" s="46">
+      <c r="E8" s="48">
         <v>44001</v>
       </c>
       <c r="F8" s="12">
         <v>0</v>
       </c>
       <c r="G8" s="32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H8" s="27"/>
     </row>
@@ -1942,16 +1987,16 @@
         <v>4</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
+        <v>26</v>
+      </c>
+      <c r="C9" s="49"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
       <c r="F9" s="12">
         <v>0</v>
       </c>
       <c r="G9" s="32" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1959,20 +2004,20 @@
         <v>5</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="48"/>
-      <c r="D10" s="46">
+        <v>27</v>
+      </c>
+      <c r="C10" s="49"/>
+      <c r="D10" s="48">
         <v>44004</v>
       </c>
-      <c r="E10" s="46">
+      <c r="E10" s="48">
         <v>44008</v>
       </c>
       <c r="F10" s="12">
         <v>0</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1980,16 +2025,16 @@
         <v>6</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="48"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
+        <v>28</v>
+      </c>
+      <c r="C11" s="49"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
       <c r="F11" s="12">
         <v>0</v>
       </c>
       <c r="G11" s="32" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H11" s="29"/>
       <c r="I11" s="29"/>
@@ -2000,20 +2045,20 @@
         <v>7</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="46">
+        <v>29</v>
+      </c>
+      <c r="C12" s="49"/>
+      <c r="D12" s="48">
         <v>44004</v>
       </c>
-      <c r="E12" s="46">
+      <c r="E12" s="48">
         <v>44008</v>
       </c>
       <c r="F12" s="12">
         <v>0</v>
       </c>
       <c r="G12" s="32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2021,16 +2066,16 @@
         <v>8</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
+        <v>30</v>
+      </c>
+      <c r="C13" s="47"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
       <c r="F13" s="12">
         <v>0</v>
       </c>
       <c r="G13" s="32" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2038,22 +2083,22 @@
         <v>9</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="47">
+        <v>31</v>
+      </c>
+      <c r="C14" s="46">
         <v>6</v>
       </c>
-      <c r="D14" s="46">
+      <c r="D14" s="48">
         <v>44011</v>
       </c>
-      <c r="E14" s="46">
+      <c r="E14" s="48">
         <v>44016</v>
       </c>
       <c r="F14" s="12">
         <v>0</v>
       </c>
       <c r="G14" s="32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -2061,16 +2106,16 @@
         <v>10</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="49"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
+        <v>32</v>
+      </c>
+      <c r="C15" s="47"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
       <c r="F15" s="12">
         <v>0</v>
       </c>
       <c r="G15" s="32" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2078,9 +2123,9 @@
         <v>9</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="47">
+        <v>33</v>
+      </c>
+      <c r="C16" s="46">
         <v>5</v>
       </c>
       <c r="D16" s="28">
@@ -2093,7 +2138,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="32" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -2101,9 +2146,9 @@
         <v>9</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="49"/>
+        <v>34</v>
+      </c>
+      <c r="C17" s="47"/>
       <c r="D17" s="28">
         <v>44025</v>
       </c>
@@ -2114,12 +2159,12 @@
         <v>0</v>
       </c>
       <c r="G17" s="32" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="30" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C18" s="22">
         <v>31</v>
@@ -2127,39 +2172,39 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="29"/>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="36" t="s">
+      <c r="D20" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="36"/>
-      <c r="F20" s="37">
+      <c r="E20" s="42"/>
+      <c r="F20" s="43">
         <f>SUM(F6:F17)/12</f>
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="29"/>
-      <c r="C21" s="36"/>
+      <c r="C21" s="42"/>
       <c r="D21" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="37"/>
+      <c r="F21" s="43"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
-      <c r="C22" s="36"/>
+      <c r="C22" s="42"/>
       <c r="D22" s="4">
         <v>43990</v>
       </c>
       <c r="E22" s="28">
         <v>44029</v>
       </c>
-      <c r="F22" s="37"/>
+      <c r="F22" s="43"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="29"/>
@@ -2169,11 +2214,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="D14:D15"/>
@@ -2188,6 +2228,11 @@
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
   </mergeCells>
   <phoneticPr fontId="31" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
se agregó el registrar al gestionar cita
</commit_message>
<xml_diff>
--- a/Requerimientos/cronograma - AMPLIACIÓN DEL SISTEMA DATA MEDIC.xlsx
+++ b/Requerimientos/cronograma - AMPLIACIÓN DEL SISTEMA DATA MEDIC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DataMedic\Requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93367365-B744-4BA7-B9E7-428E2C4558A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC7DE28-1A35-4031-AA13-D18ADBF95489}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1083,6 +1083,27 @@
     <xf numFmtId="0" fontId="33" fillId="30" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="25" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="26" fillId="27" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="25" fillId="28" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1101,37 +1122,16 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="25" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="26" fillId="27" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1459,8 +1459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1474,32 +1474,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
+      <c r="A3" s="45"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
@@ -1542,14 +1542,14 @@
       <c r="C6" s="9">
         <v>1</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="40">
         <v>43990</v>
       </c>
-      <c r="E6" s="34"/>
+      <c r="E6" s="41"/>
       <c r="F6" s="12">
         <v>1</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="G6" s="44" t="s">
         <v>21</v>
       </c>
       <c r="H6" s="26"/>
@@ -1574,7 +1574,7 @@
       <c r="F7" s="12">
         <v>0.6</v>
       </c>
-      <c r="G7" s="37"/>
+      <c r="G7" s="44"/>
     </row>
     <row r="8" spans="1:10" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
@@ -1586,14 +1586,14 @@
       <c r="C8" s="9">
         <v>1</v>
       </c>
-      <c r="D8" s="35">
+      <c r="D8" s="42">
         <v>43993</v>
       </c>
-      <c r="E8" s="36"/>
+      <c r="E8" s="43"/>
       <c r="F8" s="12">
         <v>1</v>
       </c>
-      <c r="G8" s="37"/>
+      <c r="G8" s="44"/>
       <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1615,7 +1615,7 @@
       <c r="F9" s="12">
         <v>0</v>
       </c>
-      <c r="G9" s="37"/>
+      <c r="G9" s="44"/>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
@@ -1636,7 +1636,7 @@
       <c r="F10" s="12">
         <v>0</v>
       </c>
-      <c r="G10" s="37"/>
+      <c r="G10" s="44"/>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
       <c r="J10" s="26"/>
@@ -1651,14 +1651,14 @@
       <c r="C11" s="9">
         <v>1</v>
       </c>
-      <c r="D11" s="44">
+      <c r="D11" s="38">
         <v>43997</v>
       </c>
-      <c r="E11" s="45"/>
+      <c r="E11" s="39"/>
       <c r="F11" s="12">
         <v>0</v>
       </c>
-      <c r="G11" s="37"/>
+      <c r="G11" s="44"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
@@ -1673,14 +1673,14 @@
       <c r="C12" s="9">
         <v>1</v>
       </c>
-      <c r="D12" s="44">
+      <c r="D12" s="38">
         <v>43998</v>
       </c>
-      <c r="E12" s="45"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="12">
         <v>0</v>
       </c>
-      <c r="G12" s="37"/>
+      <c r="G12" s="44"/>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
@@ -1701,7 +1701,7 @@
       <c r="F13" s="12">
         <v>0</v>
       </c>
-      <c r="G13" s="37"/>
+      <c r="G13" s="44"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -1722,7 +1722,7 @@
       <c r="F14" s="12">
         <v>0</v>
       </c>
-      <c r="G14" s="37"/>
+      <c r="G14" s="44"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
@@ -1734,14 +1734,14 @@
       <c r="C15" s="9">
         <v>1</v>
       </c>
-      <c r="D15" s="35">
+      <c r="D15" s="42">
         <v>44004</v>
       </c>
-      <c r="E15" s="36"/>
+      <c r="E15" s="43"/>
       <c r="F15" s="12">
         <v>0</v>
       </c>
-      <c r="G15" s="37"/>
+      <c r="G15" s="44"/>
     </row>
     <row r="16" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
@@ -1753,14 +1753,14 @@
       <c r="C16" s="9">
         <v>1</v>
       </c>
-      <c r="D16" s="35">
+      <c r="D16" s="42">
         <v>44005</v>
       </c>
-      <c r="E16" s="36"/>
+      <c r="E16" s="43"/>
       <c r="F16" s="12">
         <v>0</v>
       </c>
-      <c r="G16" s="37"/>
+      <c r="G16" s="44"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
@@ -1770,10 +1770,10 @@
         <v>14</v>
       </c>
       <c r="C17" s="13"/>
-      <c r="D17" s="39">
+      <c r="D17" s="33">
         <v>44006</v>
       </c>
-      <c r="E17" s="40"/>
+      <c r="E17" s="34"/>
       <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1787,39 +1787,39 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="41" t="s">
+      <c r="D20" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="41"/>
-      <c r="F20" s="43">
+      <c r="E20" s="35"/>
+      <c r="F20" s="37">
         <f>SUM(F6:F16)/11</f>
         <v>0.23636363636363636</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="10"/>
-      <c r="C21" s="42"/>
+      <c r="C21" s="36"/>
       <c r="D21" s="18" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="43"/>
+      <c r="F21" s="37"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
-      <c r="C22" s="42"/>
+      <c r="C22" s="36"/>
       <c r="D22" s="4">
         <v>43990</v>
       </c>
       <c r="E22" s="4">
         <v>44006</v>
       </c>
-      <c r="F22" s="43"/>
+      <c r="F22" s="37"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
@@ -1829,12 +1829,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="G6:G16"/>
@@ -1843,6 +1837,12 @@
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1870,32 +1870,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
+      <c r="A3" s="45"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -1927,13 +1927,13 @@
       <c r="B6" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="46">
+      <c r="C6" s="47">
         <v>5</v>
       </c>
-      <c r="D6" s="48">
+      <c r="D6" s="46">
         <v>43990</v>
       </c>
-      <c r="E6" s="48">
+      <c r="E6" s="46">
         <v>43994</v>
       </c>
       <c r="F6" s="12">
@@ -1950,9 +1950,9 @@
       <c r="B7" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
       <c r="F7" s="12">
         <v>0</v>
       </c>
@@ -1967,11 +1967,11 @@
       <c r="B8" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="48">
+      <c r="C8" s="48"/>
+      <c r="D8" s="46">
         <v>43997</v>
       </c>
-      <c r="E8" s="48">
+      <c r="E8" s="46">
         <v>44001</v>
       </c>
       <c r="F8" s="12">
@@ -1989,9 +1989,9 @@
       <c r="B9" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
       <c r="F9" s="12">
         <v>0</v>
       </c>
@@ -2006,11 +2006,11 @@
       <c r="B10" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="48">
+      <c r="C10" s="48"/>
+      <c r="D10" s="46">
         <v>44004</v>
       </c>
-      <c r="E10" s="48">
+      <c r="E10" s="46">
         <v>44008</v>
       </c>
       <c r="F10" s="12">
@@ -2027,9 +2027,9 @@
       <c r="B11" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
       <c r="F11" s="12">
         <v>0</v>
       </c>
@@ -2047,11 +2047,11 @@
       <c r="B12" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="48">
+      <c r="C12" s="48"/>
+      <c r="D12" s="46">
         <v>44004</v>
       </c>
-      <c r="E12" s="48">
+      <c r="E12" s="46">
         <v>44008</v>
       </c>
       <c r="F12" s="12">
@@ -2068,9 +2068,9 @@
       <c r="B13" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="47"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
       <c r="F13" s="12">
         <v>0</v>
       </c>
@@ -2085,13 +2085,13 @@
       <c r="B14" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="46">
+      <c r="C14" s="47">
         <v>6</v>
       </c>
-      <c r="D14" s="48">
+      <c r="D14" s="46">
         <v>44011</v>
       </c>
-      <c r="E14" s="48">
+      <c r="E14" s="46">
         <v>44016</v>
       </c>
       <c r="F14" s="12">
@@ -2108,9 +2108,9 @@
       <c r="B15" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
       <c r="F15" s="12">
         <v>0</v>
       </c>
@@ -2125,7 +2125,7 @@
       <c r="B16" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="46">
+      <c r="C16" s="47">
         <v>5</v>
       </c>
       <c r="D16" s="28">
@@ -2148,7 +2148,7 @@
       <c r="B17" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="47"/>
+      <c r="C17" s="49"/>
       <c r="D17" s="28">
         <v>44025</v>
       </c>
@@ -2172,39 +2172,39 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="29"/>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="D20" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="42"/>
-      <c r="F20" s="43">
+      <c r="E20" s="36"/>
+      <c r="F20" s="37">
         <f>SUM(F6:F17)/12</f>
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="29"/>
-      <c r="C21" s="42"/>
+      <c r="C21" s="36"/>
       <c r="D21" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="43"/>
+      <c r="F21" s="37"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
-      <c r="C22" s="42"/>
+      <c r="C22" s="36"/>
       <c r="D22" s="4">
         <v>43990</v>
       </c>
       <c r="E22" s="28">
         <v>44029</v>
       </c>
-      <c r="F22" s="43"/>
+      <c r="F22" s="37"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="29"/>
@@ -2214,6 +2214,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="D14:D15"/>
@@ -2228,11 +2233,6 @@
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
   </mergeCells>
   <phoneticPr fontId="31" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
se agregó el módulo Doctor y se agregó su mantenimiento completo doctor
</commit_message>
<xml_diff>
--- a/Requerimientos/cronograma - AMPLIACIÓN DEL SISTEMA DATA MEDIC.xlsx
+++ b/Requerimientos/cronograma - AMPLIACIÓN DEL SISTEMA DATA MEDIC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DataMedic\Requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC7DE28-1A35-4031-AA13-D18ADBF95489}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4AC3D3-E7E8-4B83-A940-C59237C8BF00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -248,8 +248,34 @@
                                        - Encapsulamiento 100%</t>
   </si>
   <si>
+    <t>Revisar el código que tiene la plantilla para los gráficos estadísticos y diseñar la página del dashboard</t>
+  </si>
+  <si>
     <r>
       <t>Agregar al usuario el consultorio al que pertenece y actualizar el mantenimiento usuario</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(LEER COMENTARIO)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Agregar el mantenimiento completo para la: 
+                                     a. Empresa ( al 100%)
+                                     b. Sede ( al 100%)
+                                     c. Consultorio ( al 100%)
+                                     d. Área ( al 100%)                          
+                                     e. Horario de trabajo(al 100%)
+                                     f. cita(al 100%)
+                                     </t>
     </r>
     <r>
       <rPr>
@@ -260,29 +286,26 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(LEER COMENTARIO)</t>
+      <t>g. Doctor(17/06/2020)</t>
     </r>
-  </si>
-  <si>
-    <t>Agregar el mantenimiento completo para la: 
-                                     a. Empresa ( al 100%)
-                                     b. Sede ( al 100%)
-                                     c. Consultorio ( al 100%)
-                                     d. Área ( al 100%)                          
-                                     e. Horario de trabajo(al 50%)
-                                     f. cita(13/06/2020)
-                                     g. otra_especialización(13/06/2020)
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 Dar acceso a los usuarios correspondiente: Super Usuario: Empresa, Gerente: Sede y Consultorio (100%)</t>
-  </si>
-  <si>
-    <t>Revisar el código que tiene la plantilla para los gráficos estadísticos y diseñar la página del dashboard</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="38" x14ac:knownFonts="1">
+  <fonts count="39" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -551,6 +574,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -995,7 +1026,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1083,6 +1114,24 @@
     <xf numFmtId="0" fontId="33" fillId="30" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="25" fillId="28" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="28" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="30" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="25" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1104,35 +1153,38 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="25" fillId="28" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="28" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="30" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="26" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="26" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="26" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="38" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1459,8 +1511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16:E16"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1474,32 +1526,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
@@ -1536,20 +1588,20 @@
       <c r="A6" s="8">
         <v>1</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="51">
         <v>1</v>
       </c>
-      <c r="D6" s="40">
+      <c r="D6" s="33">
         <v>43990</v>
       </c>
-      <c r="E6" s="41"/>
-      <c r="F6" s="12">
+      <c r="E6" s="34"/>
+      <c r="F6" s="54">
         <v>1</v>
       </c>
-      <c r="G6" s="44" t="s">
+      <c r="G6" s="37" t="s">
         <v>21</v>
       </c>
       <c r="H6" s="26"/>
@@ -1560,7 +1612,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C7" s="9">
         <v>2</v>
@@ -1572,28 +1624,28 @@
         <v>43992</v>
       </c>
       <c r="F7" s="12">
-        <v>0.6</v>
-      </c>
-      <c r="G7" s="44"/>
+        <v>0.8</v>
+      </c>
+      <c r="G7" s="37"/>
     </row>
     <row r="8" spans="1:10" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>3</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="9">
+      <c r="B8" s="50" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="51">
         <v>1</v>
       </c>
-      <c r="D8" s="42">
+      <c r="D8" s="52">
         <v>43993</v>
       </c>
-      <c r="E8" s="43"/>
-      <c r="F8" s="12">
+      <c r="E8" s="53"/>
+      <c r="F8" s="54">
         <v>1</v>
       </c>
-      <c r="G8" s="44"/>
+      <c r="G8" s="37"/>
       <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1615,28 +1667,28 @@
       <c r="F9" s="12">
         <v>0</v>
       </c>
-      <c r="G9" s="44"/>
+      <c r="G9" s="37"/>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
         <v>5</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="55">
         <v>1</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="56">
         <v>43995</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="56">
         <v>43995</v>
       </c>
-      <c r="F10" s="12">
-        <v>0</v>
-      </c>
-      <c r="G10" s="44"/>
+      <c r="F10" s="54">
+        <v>1</v>
+      </c>
+      <c r="G10" s="37"/>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
       <c r="J10" s="26"/>
@@ -1651,14 +1703,14 @@
       <c r="C11" s="9">
         <v>1</v>
       </c>
-      <c r="D11" s="38">
+      <c r="D11" s="44">
         <v>43997</v>
       </c>
-      <c r="E11" s="39"/>
+      <c r="E11" s="45"/>
       <c r="F11" s="12">
         <v>0</v>
       </c>
-      <c r="G11" s="44"/>
+      <c r="G11" s="37"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
@@ -1668,19 +1720,19 @@
         <v>7</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" s="9">
         <v>1</v>
       </c>
-      <c r="D12" s="38">
+      <c r="D12" s="44">
         <v>43998</v>
       </c>
-      <c r="E12" s="39"/>
+      <c r="E12" s="45"/>
       <c r="F12" s="12">
         <v>0</v>
       </c>
-      <c r="G12" s="44"/>
+      <c r="G12" s="37"/>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
@@ -1701,7 +1753,7 @@
       <c r="F13" s="12">
         <v>0</v>
       </c>
-      <c r="G13" s="44"/>
+      <c r="G13" s="37"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -1722,7 +1774,7 @@
       <c r="F14" s="12">
         <v>0</v>
       </c>
-      <c r="G14" s="44"/>
+      <c r="G14" s="37"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
@@ -1734,14 +1786,14 @@
       <c r="C15" s="9">
         <v>1</v>
       </c>
-      <c r="D15" s="42">
+      <c r="D15" s="35">
         <v>44004</v>
       </c>
-      <c r="E15" s="43"/>
+      <c r="E15" s="36"/>
       <c r="F15" s="12">
         <v>0</v>
       </c>
-      <c r="G15" s="44"/>
+      <c r="G15" s="37"/>
     </row>
     <row r="16" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
@@ -1753,14 +1805,14 @@
       <c r="C16" s="9">
         <v>1</v>
       </c>
-      <c r="D16" s="42">
+      <c r="D16" s="35">
         <v>44005</v>
       </c>
-      <c r="E16" s="43"/>
+      <c r="E16" s="36"/>
       <c r="F16" s="12">
         <v>0</v>
       </c>
-      <c r="G16" s="44"/>
+      <c r="G16" s="37"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
@@ -1770,10 +1822,10 @@
         <v>14</v>
       </c>
       <c r="C17" s="13"/>
-      <c r="D17" s="33">
+      <c r="D17" s="39">
         <v>44006</v>
       </c>
-      <c r="E17" s="34"/>
+      <c r="E17" s="40"/>
       <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1787,39 +1839,39 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="35" t="s">
+      <c r="D20" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="35"/>
-      <c r="F20" s="37">
+      <c r="E20" s="41"/>
+      <c r="F20" s="43">
         <f>SUM(F6:F16)/11</f>
-        <v>0.23636363636363636</v>
+        <v>0.34545454545454546</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="10"/>
-      <c r="C21" s="36"/>
+      <c r="C21" s="42"/>
       <c r="D21" s="18" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="37"/>
+      <c r="F21" s="43"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
-      <c r="C22" s="36"/>
+      <c r="C22" s="42"/>
       <c r="D22" s="4">
         <v>43990</v>
       </c>
       <c r="E22" s="4">
         <v>44006</v>
       </c>
-      <c r="F22" s="37"/>
+      <c r="F22" s="43"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
@@ -1829,6 +1881,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="G6:G16"/>
@@ -1837,12 +1895,6 @@
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1870,32 +1922,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -1927,13 +1979,13 @@
       <c r="B6" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="47">
+      <c r="C6" s="46">
         <v>5</v>
       </c>
-      <c r="D6" s="46">
+      <c r="D6" s="48">
         <v>43990</v>
       </c>
-      <c r="E6" s="46">
+      <c r="E6" s="48">
         <v>43994</v>
       </c>
       <c r="F6" s="12">
@@ -1950,9 +2002,9 @@
       <c r="B7" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
       <c r="F7" s="12">
         <v>0</v>
       </c>
@@ -1967,11 +2019,11 @@
       <c r="B8" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="48"/>
-      <c r="D8" s="46">
+      <c r="C8" s="49"/>
+      <c r="D8" s="48">
         <v>43997</v>
       </c>
-      <c r="E8" s="46">
+      <c r="E8" s="48">
         <v>44001</v>
       </c>
       <c r="F8" s="12">
@@ -1989,9 +2041,9 @@
       <c r="B9" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
       <c r="F9" s="12">
         <v>0</v>
       </c>
@@ -2006,11 +2058,11 @@
       <c r="B10" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="48"/>
-      <c r="D10" s="46">
+      <c r="C10" s="49"/>
+      <c r="D10" s="48">
         <v>44004</v>
       </c>
-      <c r="E10" s="46">
+      <c r="E10" s="48">
         <v>44008</v>
       </c>
       <c r="F10" s="12">
@@ -2027,9 +2079,9 @@
       <c r="B11" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="48"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
       <c r="F11" s="12">
         <v>0</v>
       </c>
@@ -2047,11 +2099,11 @@
       <c r="B12" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="46">
+      <c r="C12" s="49"/>
+      <c r="D12" s="48">
         <v>44004</v>
       </c>
-      <c r="E12" s="46">
+      <c r="E12" s="48">
         <v>44008</v>
       </c>
       <c r="F12" s="12">
@@ -2068,9 +2120,9 @@
       <c r="B13" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
       <c r="F13" s="12">
         <v>0</v>
       </c>
@@ -2085,13 +2137,13 @@
       <c r="B14" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="47">
+      <c r="C14" s="46">
         <v>6</v>
       </c>
-      <c r="D14" s="46">
+      <c r="D14" s="48">
         <v>44011</v>
       </c>
-      <c r="E14" s="46">
+      <c r="E14" s="48">
         <v>44016</v>
       </c>
       <c r="F14" s="12">
@@ -2108,9 +2160,9 @@
       <c r="B15" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="49"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
       <c r="F15" s="12">
         <v>0</v>
       </c>
@@ -2125,7 +2177,7 @@
       <c r="B16" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="47">
+      <c r="C16" s="46">
         <v>5</v>
       </c>
       <c r="D16" s="28">
@@ -2148,7 +2200,7 @@
       <c r="B17" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="49"/>
+      <c r="C17" s="47"/>
       <c r="D17" s="28">
         <v>44025</v>
       </c>
@@ -2172,39 +2224,39 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="29"/>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="36" t="s">
+      <c r="D20" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="36"/>
-      <c r="F20" s="37">
+      <c r="E20" s="42"/>
+      <c r="F20" s="43">
         <f>SUM(F6:F17)/12</f>
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="29"/>
-      <c r="C21" s="36"/>
+      <c r="C21" s="42"/>
       <c r="D21" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="37"/>
+      <c r="F21" s="43"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
-      <c r="C22" s="36"/>
+      <c r="C22" s="42"/>
       <c r="D22" s="4">
         <v>43990</v>
       </c>
       <c r="E22" s="28">
         <v>44029</v>
       </c>
-      <c r="F22" s="37"/>
+      <c r="F22" s="43"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="29"/>
@@ -2214,11 +2266,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="D14:D15"/>
@@ -2233,6 +2280,11 @@
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
   </mergeCells>
   <phoneticPr fontId="31" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
se agregó el módulo y mantenimiento de doctor especialidad
</commit_message>
<xml_diff>
--- a/Requerimientos/cronograma - AMPLIACIÓN DEL SISTEMA DATA MEDIC.xlsx
+++ b/Requerimientos/cronograma - AMPLIACIÓN DEL SISTEMA DATA MEDIC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DataMedic\Requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4AC3D3-E7E8-4B83-A940-C59237C8BF00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B428F17-D1C2-494F-961C-B7DAB1E4B5FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -126,31 +126,19 @@
     <t>Inicio</t>
   </si>
   <si>
-    <t>Mostrar dentro del sistema, como página principal al: Gerente: Dashboard, Doctor: Citas confirmadas, Cliente: registrar sus citas y super usuario: logs.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Actualizar e implementar los nuevos logs que requiere el sistema. </t>
   </si>
   <si>
     <t>Hacer pruebas para validar el funcionamiento de las actualizaciones.</t>
   </si>
   <si>
-    <t>Corregir los erroes que pueda tener las nuevas actualizaciones</t>
-  </si>
-  <si>
     <t>Entrega</t>
   </si>
   <si>
     <t>AMPLIACIÓN Y MEJORAS DEL SISTEMA CLÍNICO</t>
   </si>
   <si>
-    <t>Actualizar:  La información general en la historia clínica(se investigará y se definirá un estandar general) y su mantenimiento</t>
-  </si>
-  <si>
     <t>Mostrar como página de inicio el formulario de iniciar sesión con su respectivo fondo. Se agregará el diseño inicial del horario de citas(index) a la página gestionarCitas</t>
-  </si>
-  <si>
-    <t>Implementar los reportes que tendrá el dashboard: Qué citas tengo y en que consultorio, Próximas citas y Qué consultorios tiene más citas.</t>
   </si>
   <si>
     <t>Total de días</t>
@@ -267,6 +255,18 @@
     </r>
   </si>
   <si>
+    <t>Actualizar:  La información general en la historia clínica(se investigará y se definirá un estandar general al 100% para el 18/06/2020) y su mantenimiento al 20 % al 18/06/2020 y al 100 % al 19/06/2020</t>
+  </si>
+  <si>
+    <t>Mostrar dentro del sistema, como página principal al: Gerente: Dashboard (falta), Doctor: Citas confirmadas, Cliente: registrar sus citas y super usuario: logs.</t>
+  </si>
+  <si>
+    <t>Implementar los reportes que tendrá el dashboard: Qué citas tengo y en que consultorio, Próximas citas y Qué consultorios tiene más citas, entre otras necesarias.</t>
+  </si>
+  <si>
+    <t>Subir a la web el proyecto y hacer pruebas</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Agregar el mantenimiento completo para la: 
                                      a. Empresa ( al 100%)
@@ -279,6 +279,16 @@
     </r>
     <r>
       <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">g. Doctor(al 100%)
+</t>
+    </r>
+    <r>
+      <rPr>
         <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
@@ -286,7 +296,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>g. Doctor(17/06/2020)</t>
+      <t xml:space="preserve">                                     h. DoctorEspecialidad(18/06/2020)</t>
     </r>
     <r>
       <rPr>
@@ -305,7 +315,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="39" x14ac:knownFonts="1">
+  <fonts count="40" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -582,6 +592,12 @@
       <i/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1026,7 +1042,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1114,6 +1130,39 @@
     <xf numFmtId="0" fontId="33" fillId="30" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="26" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="26" fillId="27" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="25" fillId="28" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1132,59 +1181,29 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="25" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="26" fillId="27" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="25" fillId="26" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="26" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="26" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="26" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="26" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="38" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="14" fontId="38" fillId="26" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="38" fillId="26" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1511,8 +1530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1526,32 +1545,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="A2" s="49" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
+      <c r="A3" s="49"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
@@ -1581,33 +1600,33 @@
         <v>5</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>1</v>
       </c>
-      <c r="B6" s="50" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="51">
+      <c r="B6" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="34">
         <v>1</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="44">
         <v>43990</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="54">
+      <c r="E6" s="45"/>
+      <c r="F6" s="35">
         <v>1</v>
       </c>
-      <c r="G6" s="37" t="s">
-        <v>21</v>
+      <c r="G6" s="48" t="s">
+        <v>17</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
     </row>
-    <row r="7" spans="1:10" s="7" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="7" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>2</v>
       </c>
@@ -1626,26 +1645,26 @@
       <c r="F7" s="12">
         <v>0.8</v>
       </c>
-      <c r="G7" s="37"/>
+      <c r="G7" s="48"/>
     </row>
     <row r="8" spans="1:10" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>3</v>
       </c>
-      <c r="B8" s="50" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="51">
+      <c r="B8" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="34">
         <v>1</v>
       </c>
-      <c r="D8" s="52">
+      <c r="D8" s="50">
         <v>43993</v>
       </c>
-      <c r="E8" s="53"/>
-      <c r="F8" s="54">
+      <c r="E8" s="51"/>
+      <c r="F8" s="35">
         <v>1</v>
       </c>
-      <c r="G8" s="37"/>
+      <c r="G8" s="48"/>
       <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1653,42 +1672,40 @@
         <v>4</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="C9" s="17">
         <v>2</v>
       </c>
       <c r="D9" s="19">
-        <v>43993</v>
+        <v>44000</v>
       </c>
       <c r="E9" s="19">
-        <v>43994</v>
+        <v>44001</v>
       </c>
       <c r="F9" s="12">
         <v>0</v>
       </c>
-      <c r="G9" s="37"/>
+      <c r="G9" s="48"/>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
         <v>5</v>
       </c>
-      <c r="B10" s="50" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="55">
+      <c r="B10" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="36">
         <v>1</v>
       </c>
       <c r="D10" s="56">
-        <v>43995</v>
-      </c>
-      <c r="E10" s="56">
-        <v>43995</v>
-      </c>
-      <c r="F10" s="54">
-        <v>1</v>
-      </c>
-      <c r="G10" s="37"/>
+        <v>44001</v>
+      </c>
+      <c r="E10" s="57"/>
+      <c r="F10" s="35">
+        <v>0.8</v>
+      </c>
+      <c r="G10" s="48"/>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
       <c r="J10" s="26"/>
@@ -1698,19 +1715,19 @@
         <v>6</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="C11" s="9">
         <v>1</v>
       </c>
-      <c r="D11" s="44">
-        <v>43997</v>
-      </c>
-      <c r="E11" s="45"/>
+      <c r="D11" s="42">
+        <v>44002</v>
+      </c>
+      <c r="E11" s="43"/>
       <c r="F11" s="12">
-        <v>0</v>
-      </c>
-      <c r="G11" s="37"/>
+        <v>0.8</v>
+      </c>
+      <c r="G11" s="48"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
@@ -1720,117 +1737,117 @@
         <v>7</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C12" s="9">
         <v>1</v>
       </c>
-      <c r="D12" s="44">
-        <v>43998</v>
-      </c>
-      <c r="E12" s="45"/>
+      <c r="D12" s="42">
+        <v>44003</v>
+      </c>
+      <c r="E12" s="43"/>
       <c r="F12" s="12">
         <v>0</v>
       </c>
-      <c r="G12" s="37"/>
+      <c r="G12" s="48"/>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>8</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="C13" s="9">
         <v>2</v>
       </c>
       <c r="D13" s="19">
-        <v>43999</v>
+        <v>44004</v>
       </c>
       <c r="E13" s="19">
-        <v>44000</v>
+        <v>44005</v>
       </c>
       <c r="F13" s="12">
         <v>0</v>
       </c>
-      <c r="G13" s="37"/>
+      <c r="G13" s="48"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>9</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="1">
         <v>2</v>
       </c>
       <c r="D14" s="19">
-        <v>44001</v>
+        <v>44006</v>
       </c>
       <c r="E14" s="19">
-        <v>44002</v>
+        <v>44007</v>
       </c>
       <c r="F14" s="12">
         <v>0</v>
       </c>
-      <c r="G14" s="37"/>
+      <c r="G14" s="48"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>10</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" s="9">
         <v>1</v>
       </c>
-      <c r="D15" s="35">
-        <v>44004</v>
-      </c>
-      <c r="E15" s="36"/>
+      <c r="D15" s="46">
+        <v>44008</v>
+      </c>
+      <c r="E15" s="47"/>
       <c r="F15" s="12">
         <v>0</v>
       </c>
-      <c r="G15" s="37"/>
+      <c r="G15" s="48"/>
     </row>
     <row r="16" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>11</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C16" s="9">
         <v>1</v>
       </c>
-      <c r="D16" s="35">
-        <v>44005</v>
-      </c>
-      <c r="E16" s="36"/>
+      <c r="D16" s="46">
+        <v>44009</v>
+      </c>
+      <c r="E16" s="47"/>
       <c r="F16" s="12">
         <v>0</v>
       </c>
-      <c r="G16" s="37"/>
+      <c r="G16" s="48"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>12</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C17" s="13"/>
-      <c r="D17" s="39">
-        <v>44006</v>
-      </c>
-      <c r="E17" s="40"/>
+      <c r="D17" s="37">
+        <v>44011</v>
+      </c>
+      <c r="E17" s="38"/>
       <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="21" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C18" s="22">
         <f>SUM(C6:C16)</f>
@@ -1839,39 +1856,39 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="41" t="s">
+      <c r="D20" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="41"/>
-      <c r="F20" s="43">
+      <c r="E20" s="39"/>
+      <c r="F20" s="41">
         <f>SUM(F6:F16)/11</f>
-        <v>0.34545454545454546</v>
+        <v>0.39999999999999997</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="10"/>
-      <c r="C21" s="42"/>
+      <c r="C21" s="40"/>
       <c r="D21" s="18" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="43"/>
+      <c r="F21" s="41"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
-      <c r="C22" s="42"/>
+      <c r="C22" s="40"/>
       <c r="D22" s="4">
         <v>43990</v>
       </c>
       <c r="E22" s="4">
         <v>44006</v>
       </c>
-      <c r="F22" s="43"/>
+      <c r="F22" s="41"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
@@ -1880,13 +1897,7 @@
       <c r="B24" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
+  <mergeCells count="15">
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="G6:G16"/>
@@ -1895,6 +1906,13 @@
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1922,32 +1940,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="A2" s="49" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
+      <c r="A3" s="49"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -1969,7 +1987,7 @@
         <v>5</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -1977,22 +1995,22 @@
         <v>1</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="46">
+        <v>33</v>
+      </c>
+      <c r="C6" s="53">
         <v>5</v>
       </c>
-      <c r="D6" s="48">
+      <c r="D6" s="52">
         <v>43990</v>
       </c>
-      <c r="E6" s="48">
+      <c r="E6" s="52">
         <v>43994</v>
       </c>
       <c r="F6" s="12">
         <v>0.4</v>
       </c>
       <c r="G6" s="32" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2000,16 +2018,16 @@
         <v>2</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
+        <v>21</v>
+      </c>
+      <c r="C7" s="54"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
       <c r="F7" s="12">
         <v>0</v>
       </c>
       <c r="G7" s="32" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2017,20 +2035,20 @@
         <v>3</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="48">
+        <v>20</v>
+      </c>
+      <c r="C8" s="54"/>
+      <c r="D8" s="52">
         <v>43997</v>
       </c>
-      <c r="E8" s="48">
+      <c r="E8" s="52">
         <v>44001</v>
       </c>
       <c r="F8" s="12">
         <v>0</v>
       </c>
       <c r="G8" s="32" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H8" s="27"/>
     </row>
@@ -2039,16 +2057,16 @@
         <v>4</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
+        <v>22</v>
+      </c>
+      <c r="C9" s="54"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
       <c r="F9" s="12">
         <v>0</v>
       </c>
       <c r="G9" s="32" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2056,20 +2074,20 @@
         <v>5</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="48">
+        <v>23</v>
+      </c>
+      <c r="C10" s="54"/>
+      <c r="D10" s="52">
         <v>44004</v>
       </c>
-      <c r="E10" s="48">
+      <c r="E10" s="52">
         <v>44008</v>
       </c>
       <c r="F10" s="12">
         <v>0</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2077,16 +2095,16 @@
         <v>6</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
+        <v>24</v>
+      </c>
+      <c r="C11" s="54"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
       <c r="F11" s="12">
         <v>0</v>
       </c>
       <c r="G11" s="32" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H11" s="29"/>
       <c r="I11" s="29"/>
@@ -2097,20 +2115,20 @@
         <v>7</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="48">
+        <v>25</v>
+      </c>
+      <c r="C12" s="54"/>
+      <c r="D12" s="52">
         <v>44004</v>
       </c>
-      <c r="E12" s="48">
+      <c r="E12" s="52">
         <v>44008</v>
       </c>
       <c r="F12" s="12">
         <v>0</v>
       </c>
       <c r="G12" s="32" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2118,16 +2136,16 @@
         <v>8</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="47"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
+        <v>26</v>
+      </c>
+      <c r="C13" s="55"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
       <c r="F13" s="12">
         <v>0</v>
       </c>
       <c r="G13" s="32" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2135,22 +2153,22 @@
         <v>9</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="46">
+        <v>27</v>
+      </c>
+      <c r="C14" s="53">
         <v>6</v>
       </c>
-      <c r="D14" s="48">
+      <c r="D14" s="52">
         <v>44011</v>
       </c>
-      <c r="E14" s="48">
+      <c r="E14" s="52">
         <v>44016</v>
       </c>
       <c r="F14" s="12">
         <v>0</v>
       </c>
       <c r="G14" s="32" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -2158,16 +2176,16 @@
         <v>10</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
+        <v>28</v>
+      </c>
+      <c r="C15" s="55"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
       <c r="F15" s="12">
         <v>0</v>
       </c>
       <c r="G15" s="32" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2175,9 +2193,9 @@
         <v>9</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="46">
+        <v>29</v>
+      </c>
+      <c r="C16" s="53">
         <v>5</v>
       </c>
       <c r="D16" s="28">
@@ -2190,7 +2208,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="32" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -2198,9 +2216,9 @@
         <v>9</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="47"/>
+        <v>30</v>
+      </c>
+      <c r="C17" s="55"/>
       <c r="D17" s="28">
         <v>44025</v>
       </c>
@@ -2211,12 +2229,12 @@
         <v>0</v>
       </c>
       <c r="G17" s="32" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="30" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C18" s="22">
         <v>31</v>
@@ -2224,39 +2242,39 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="29"/>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="D20" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="42"/>
-      <c r="F20" s="43">
+      <c r="E20" s="40"/>
+      <c r="F20" s="41">
         <f>SUM(F6:F17)/12</f>
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="29"/>
-      <c r="C21" s="42"/>
+      <c r="C21" s="40"/>
       <c r="D21" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="43"/>
+      <c r="F21" s="41"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
-      <c r="C22" s="42"/>
+      <c r="C22" s="40"/>
       <c r="D22" s="4">
         <v>43990</v>
       </c>
       <c r="E22" s="28">
         <v>44029</v>
       </c>
-      <c r="F22" s="43"/>
+      <c r="F22" s="41"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="29"/>
@@ -2266,6 +2284,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="D14:D15"/>
@@ -2280,11 +2303,6 @@
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
   </mergeCells>
   <phoneticPr fontId="31" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
se agregó el fondo y el inicio de sesión en la página index.php
</commit_message>
<xml_diff>
--- a/Requerimientos/cronograma - AMPLIACIÓN DEL SISTEMA DATA MEDIC.xlsx
+++ b/Requerimientos/cronograma - AMPLIACIÓN DEL SISTEMA DATA MEDIC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DataMedic\Requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B428F17-D1C2-494F-961C-B7DAB1E4B5FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E34AD47-C66E-4AF5-BC0A-36569B45EDBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -289,24 +289,13 @@
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                                     h. DoctorEspecialidad(18/06/2020)</t>
-    </r>
-    <r>
-      <rPr>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">
+      <t xml:space="preserve">                                     h. DoctorEspecialidad(al 100%)
 Dar acceso a los usuarios correspondiente: Super Usuario: Empresa, Gerente: Sede y Consultorio (100%)</t>
     </r>
   </si>
@@ -315,7 +304,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="40" x14ac:knownFonts="1">
+  <fonts count="39" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -579,14 +568,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <i/>
@@ -1142,6 +1123,36 @@
     <xf numFmtId="0" fontId="26" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="25" fillId="28" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="28" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="30" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="26" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="26" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="37" fillId="26" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="37" fillId="26" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="25" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1163,46 +1174,16 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="25" fillId="28" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="28" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="30" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="26" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="26" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="38" fillId="26" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="38" fillId="26" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1530,8 +1511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1545,32 +1526,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="49"/>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
@@ -1613,14 +1594,14 @@
       <c r="C6" s="34">
         <v>1</v>
       </c>
-      <c r="D6" s="44">
+      <c r="D6" s="37">
         <v>43990</v>
       </c>
-      <c r="E6" s="45"/>
+      <c r="E6" s="38"/>
       <c r="F6" s="35">
         <v>1</v>
       </c>
-      <c r="G6" s="48" t="s">
+      <c r="G6" s="41" t="s">
         <v>17</v>
       </c>
       <c r="H6" s="26"/>
@@ -1643,9 +1624,9 @@
         <v>43992</v>
       </c>
       <c r="F7" s="12">
-        <v>0.8</v>
-      </c>
-      <c r="G7" s="48"/>
+        <v>1</v>
+      </c>
+      <c r="G7" s="41"/>
     </row>
     <row r="8" spans="1:10" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
@@ -1657,14 +1638,14 @@
       <c r="C8" s="34">
         <v>1</v>
       </c>
-      <c r="D8" s="50">
+      <c r="D8" s="43">
         <v>43993</v>
       </c>
-      <c r="E8" s="51"/>
+      <c r="E8" s="44"/>
       <c r="F8" s="35">
         <v>1</v>
       </c>
-      <c r="G8" s="48"/>
+      <c r="G8" s="41"/>
       <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1686,7 +1667,7 @@
       <c r="F9" s="12">
         <v>0</v>
       </c>
-      <c r="G9" s="48"/>
+      <c r="G9" s="41"/>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
@@ -1698,14 +1679,14 @@
       <c r="C10" s="36">
         <v>1</v>
       </c>
-      <c r="D10" s="56">
+      <c r="D10" s="45">
         <v>44001</v>
       </c>
-      <c r="E10" s="57"/>
+      <c r="E10" s="46"/>
       <c r="F10" s="35">
         <v>0.8</v>
       </c>
-      <c r="G10" s="48"/>
+      <c r="G10" s="41"/>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
       <c r="J10" s="26"/>
@@ -1720,14 +1701,14 @@
       <c r="C11" s="9">
         <v>1</v>
       </c>
-      <c r="D11" s="42">
+      <c r="D11" s="52">
         <v>44002</v>
       </c>
-      <c r="E11" s="43"/>
+      <c r="E11" s="53"/>
       <c r="F11" s="12">
         <v>0.8</v>
       </c>
-      <c r="G11" s="48"/>
+      <c r="G11" s="41"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
@@ -1742,14 +1723,14 @@
       <c r="C12" s="9">
         <v>1</v>
       </c>
-      <c r="D12" s="42">
+      <c r="D12" s="52">
         <v>44003</v>
       </c>
-      <c r="E12" s="43"/>
+      <c r="E12" s="53"/>
       <c r="F12" s="12">
         <v>0</v>
       </c>
-      <c r="G12" s="48"/>
+      <c r="G12" s="41"/>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
@@ -1770,7 +1751,7 @@
       <c r="F13" s="12">
         <v>0</v>
       </c>
-      <c r="G13" s="48"/>
+      <c r="G13" s="41"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -1791,7 +1772,7 @@
       <c r="F14" s="12">
         <v>0</v>
       </c>
-      <c r="G14" s="48"/>
+      <c r="G14" s="41"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
@@ -1803,14 +1784,14 @@
       <c r="C15" s="9">
         <v>1</v>
       </c>
-      <c r="D15" s="46">
+      <c r="D15" s="39">
         <v>44008</v>
       </c>
-      <c r="E15" s="47"/>
+      <c r="E15" s="40"/>
       <c r="F15" s="12">
         <v>0</v>
       </c>
-      <c r="G15" s="48"/>
+      <c r="G15" s="41"/>
     </row>
     <row r="16" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
@@ -1822,14 +1803,14 @@
       <c r="C16" s="9">
         <v>1</v>
       </c>
-      <c r="D16" s="46">
+      <c r="D16" s="39">
         <v>44009</v>
       </c>
-      <c r="E16" s="47"/>
+      <c r="E16" s="40"/>
       <c r="F16" s="12">
         <v>0</v>
       </c>
-      <c r="G16" s="48"/>
+      <c r="G16" s="41"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
@@ -1839,10 +1820,10 @@
         <v>12</v>
       </c>
       <c r="C17" s="13"/>
-      <c r="D17" s="37">
+      <c r="D17" s="47">
         <v>44011</v>
       </c>
-      <c r="E17" s="38"/>
+      <c r="E17" s="48"/>
       <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1856,39 +1837,39 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
-      <c r="C20" s="40" t="s">
+      <c r="C20" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="39" t="s">
+      <c r="D20" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="39"/>
-      <c r="F20" s="41">
+      <c r="E20" s="49"/>
+      <c r="F20" s="51">
         <f>SUM(F6:F16)/11</f>
-        <v>0.39999999999999997</v>
+        <v>0.41818181818181815</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="10"/>
-      <c r="C21" s="40"/>
+      <c r="C21" s="50"/>
       <c r="D21" s="18" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="41"/>
+      <c r="F21" s="51"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
-      <c r="C22" s="40"/>
+      <c r="C22" s="50"/>
       <c r="D22" s="4">
         <v>43990</v>
       </c>
       <c r="E22" s="4">
         <v>44006</v>
       </c>
-      <c r="F22" s="41"/>
+      <c r="F22" s="51"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
@@ -1898,6 +1879,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="G6:G16"/>
@@ -1907,12 +1894,6 @@
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1940,32 +1921,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="49"/>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -1997,13 +1978,13 @@
       <c r="B6" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="53">
+      <c r="C6" s="54">
         <v>5</v>
       </c>
-      <c r="D6" s="52">
+      <c r="D6" s="56">
         <v>43990</v>
       </c>
-      <c r="E6" s="52">
+      <c r="E6" s="56">
         <v>43994</v>
       </c>
       <c r="F6" s="12">
@@ -2020,9 +2001,9 @@
       <c r="B7" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="54"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
       <c r="F7" s="12">
         <v>0</v>
       </c>
@@ -2037,11 +2018,11 @@
       <c r="B8" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="54"/>
-      <c r="D8" s="52">
+      <c r="C8" s="57"/>
+      <c r="D8" s="56">
         <v>43997</v>
       </c>
-      <c r="E8" s="52">
+      <c r="E8" s="56">
         <v>44001</v>
       </c>
       <c r="F8" s="12">
@@ -2059,9 +2040,9 @@
       <c r="B9" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
       <c r="F9" s="12">
         <v>0</v>
       </c>
@@ -2076,11 +2057,11 @@
       <c r="B10" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="54"/>
-      <c r="D10" s="52">
+      <c r="C10" s="57"/>
+      <c r="D10" s="56">
         <v>44004</v>
       </c>
-      <c r="E10" s="52">
+      <c r="E10" s="56">
         <v>44008</v>
       </c>
       <c r="F10" s="12">
@@ -2097,9 +2078,9 @@
       <c r="B11" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="54"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
       <c r="F11" s="12">
         <v>0</v>
       </c>
@@ -2117,11 +2098,11 @@
       <c r="B12" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="54"/>
-      <c r="D12" s="52">
+      <c r="C12" s="57"/>
+      <c r="D12" s="56">
         <v>44004</v>
       </c>
-      <c r="E12" s="52">
+      <c r="E12" s="56">
         <v>44008</v>
       </c>
       <c r="F12" s="12">
@@ -2139,8 +2120,8 @@
         <v>26</v>
       </c>
       <c r="C13" s="55"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
       <c r="F13" s="12">
         <v>0</v>
       </c>
@@ -2155,13 +2136,13 @@
       <c r="B14" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="53">
+      <c r="C14" s="54">
         <v>6</v>
       </c>
-      <c r="D14" s="52">
+      <c r="D14" s="56">
         <v>44011</v>
       </c>
-      <c r="E14" s="52">
+      <c r="E14" s="56">
         <v>44016</v>
       </c>
       <c r="F14" s="12">
@@ -2179,8 +2160,8 @@
         <v>28</v>
       </c>
       <c r="C15" s="55"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
       <c r="F15" s="12">
         <v>0</v>
       </c>
@@ -2195,7 +2176,7 @@
       <c r="B16" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="53">
+      <c r="C16" s="54">
         <v>5</v>
       </c>
       <c r="D16" s="28">
@@ -2242,39 +2223,39 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="29"/>
-      <c r="C20" s="40" t="s">
+      <c r="C20" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="40" t="s">
+      <c r="D20" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="40"/>
-      <c r="F20" s="41">
+      <c r="E20" s="50"/>
+      <c r="F20" s="51">
         <f>SUM(F6:F17)/12</f>
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="29"/>
-      <c r="C21" s="40"/>
+      <c r="C21" s="50"/>
       <c r="D21" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="41"/>
+      <c r="F21" s="51"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
-      <c r="C22" s="40"/>
+      <c r="C22" s="50"/>
       <c r="D22" s="4">
         <v>43990</v>
       </c>
       <c r="E22" s="28">
         <v>44029</v>
       </c>
-      <c r="F22" s="41"/>
+      <c r="F22" s="51"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="29"/>
@@ -2284,11 +2265,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="D14:D15"/>
@@ -2303,6 +2279,11 @@
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
   </mergeCells>
   <phoneticPr fontId="31" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
se solucionó el problema de la historia clinica general
</commit_message>
<xml_diff>
--- a/Requerimientos/cronograma - AMPLIACIÓN DEL SISTEMA DATA MEDIC.xlsx
+++ b/Requerimientos/cronograma - AMPLIACIÓN DEL SISTEMA DATA MEDIC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DataMedic\Requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E34AD47-C66E-4AF5-BC0A-36569B45EDBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9A8A4C-F16D-40A4-B21E-98D18D13E07C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -744,7 +744,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -974,6 +974,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1023,7 +1045,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1123,6 +1145,27 @@
     <xf numFmtId="0" fontId="26" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="25" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="26" fillId="27" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="25" fillId="28" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1153,37 +1196,28 @@
     <xf numFmtId="14" fontId="37" fillId="26" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="25" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="26" fillId="27" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1512,7 +1546,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1526,32 +1560,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="42"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
+      <c r="A3" s="49"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
@@ -1594,14 +1628,14 @@
       <c r="C6" s="34">
         <v>1</v>
       </c>
-      <c r="D6" s="37">
+      <c r="D6" s="44">
         <v>43990</v>
       </c>
-      <c r="E6" s="38"/>
+      <c r="E6" s="45"/>
       <c r="F6" s="35">
         <v>1</v>
       </c>
-      <c r="G6" s="41" t="s">
+      <c r="G6" s="48" t="s">
         <v>17</v>
       </c>
       <c r="H6" s="26"/>
@@ -1626,7 +1660,7 @@
       <c r="F7" s="12">
         <v>1</v>
       </c>
-      <c r="G7" s="41"/>
+      <c r="G7" s="48"/>
     </row>
     <row r="8" spans="1:10" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
@@ -1638,14 +1672,14 @@
       <c r="C8" s="34">
         <v>1</v>
       </c>
-      <c r="D8" s="43">
+      <c r="D8" s="50">
         <v>43993</v>
       </c>
-      <c r="E8" s="44"/>
+      <c r="E8" s="51"/>
       <c r="F8" s="35">
         <v>1</v>
       </c>
-      <c r="G8" s="41"/>
+      <c r="G8" s="48"/>
       <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1665,9 +1699,9 @@
         <v>44001</v>
       </c>
       <c r="F9" s="12">
-        <v>0</v>
-      </c>
-      <c r="G9" s="41"/>
+        <v>1</v>
+      </c>
+      <c r="G9" s="48"/>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
@@ -1679,14 +1713,14 @@
       <c r="C10" s="36">
         <v>1</v>
       </c>
-      <c r="D10" s="45">
+      <c r="D10" s="52">
         <v>44001</v>
       </c>
-      <c r="E10" s="46"/>
+      <c r="E10" s="53"/>
       <c r="F10" s="35">
-        <v>0.8</v>
-      </c>
-      <c r="G10" s="41"/>
+        <v>1</v>
+      </c>
+      <c r="G10" s="48"/>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
       <c r="J10" s="26"/>
@@ -1698,17 +1732,17 @@
       <c r="B11" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="60">
         <v>1</v>
       </c>
-      <c r="D11" s="52">
+      <c r="D11" s="42">
         <v>44002</v>
       </c>
-      <c r="E11" s="53"/>
+      <c r="E11" s="43"/>
       <c r="F11" s="12">
         <v>0.8</v>
       </c>
-      <c r="G11" s="41"/>
+      <c r="G11" s="48"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
@@ -1720,17 +1754,13 @@
       <c r="B12" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="9">
-        <v>1</v>
-      </c>
-      <c r="D12" s="52">
-        <v>44003</v>
-      </c>
-      <c r="E12" s="53"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="59"/>
       <c r="F12" s="12">
         <v>0</v>
       </c>
-      <c r="G12" s="41"/>
+      <c r="G12" s="48"/>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
@@ -1751,7 +1781,7 @@
       <c r="F13" s="12">
         <v>0</v>
       </c>
-      <c r="G13" s="41"/>
+      <c r="G13" s="48"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -1772,7 +1802,7 @@
       <c r="F14" s="12">
         <v>0</v>
       </c>
-      <c r="G14" s="41"/>
+      <c r="G14" s="48"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
@@ -1784,14 +1814,14 @@
       <c r="C15" s="9">
         <v>1</v>
       </c>
-      <c r="D15" s="39">
+      <c r="D15" s="46">
         <v>44008</v>
       </c>
-      <c r="E15" s="40"/>
+      <c r="E15" s="47"/>
       <c r="F15" s="12">
         <v>0</v>
       </c>
-      <c r="G15" s="41"/>
+      <c r="G15" s="48"/>
     </row>
     <row r="16" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
@@ -1803,14 +1833,14 @@
       <c r="C16" s="9">
         <v>1</v>
       </c>
-      <c r="D16" s="39">
+      <c r="D16" s="46">
         <v>44009</v>
       </c>
-      <c r="E16" s="40"/>
+      <c r="E16" s="47"/>
       <c r="F16" s="12">
         <v>0</v>
       </c>
-      <c r="G16" s="41"/>
+      <c r="G16" s="48"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
@@ -1820,10 +1850,10 @@
         <v>12</v>
       </c>
       <c r="C17" s="13"/>
-      <c r="D17" s="47">
+      <c r="D17" s="37">
         <v>44011</v>
       </c>
-      <c r="E17" s="48"/>
+      <c r="E17" s="38"/>
       <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1832,44 +1862,44 @@
       </c>
       <c r="C18" s="22">
         <f>SUM(C6:C16)</f>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
-      <c r="C20" s="50" t="s">
+      <c r="C20" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="49" t="s">
+      <c r="D20" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="49"/>
-      <c r="F20" s="51">
+      <c r="E20" s="39"/>
+      <c r="F20" s="41">
         <f>SUM(F6:F16)/11</f>
-        <v>0.41818181818181815</v>
+        <v>0.52727272727272723</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="10"/>
-      <c r="C21" s="50"/>
+      <c r="C21" s="40"/>
       <c r="D21" s="18" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="51"/>
+      <c r="F21" s="41"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
-      <c r="C22" s="50"/>
+      <c r="C22" s="40"/>
       <c r="D22" s="4">
         <v>43990</v>
       </c>
       <c r="E22" s="4">
         <v>44006</v>
       </c>
-      <c r="F22" s="51"/>
+      <c r="F22" s="41"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
@@ -1879,12 +1909,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="G6:G16"/>
@@ -1894,6 +1918,12 @@
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="F20:F22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1921,32 +1951,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="42"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
+      <c r="A3" s="49"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -1978,13 +2008,13 @@
       <c r="B6" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="54">
+      <c r="C6" s="55">
         <v>5</v>
       </c>
-      <c r="D6" s="56">
+      <c r="D6" s="54">
         <v>43990</v>
       </c>
-      <c r="E6" s="56">
+      <c r="E6" s="54">
         <v>43994</v>
       </c>
       <c r="F6" s="12">
@@ -2001,9 +2031,9 @@
       <c r="B7" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="57"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
       <c r="F7" s="12">
         <v>0</v>
       </c>
@@ -2018,11 +2048,11 @@
       <c r="B8" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="57"/>
-      <c r="D8" s="56">
+      <c r="C8" s="56"/>
+      <c r="D8" s="54">
         <v>43997</v>
       </c>
-      <c r="E8" s="56">
+      <c r="E8" s="54">
         <v>44001</v>
       </c>
       <c r="F8" s="12">
@@ -2040,9 +2070,9 @@
       <c r="B9" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="57"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
       <c r="F9" s="12">
         <v>0</v>
       </c>
@@ -2057,11 +2087,11 @@
       <c r="B10" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="56">
+      <c r="C10" s="56"/>
+      <c r="D10" s="54">
         <v>44004</v>
       </c>
-      <c r="E10" s="56">
+      <c r="E10" s="54">
         <v>44008</v>
       </c>
       <c r="F10" s="12">
@@ -2078,9 +2108,9 @@
       <c r="B11" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="57"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
       <c r="F11" s="12">
         <v>0</v>
       </c>
@@ -2098,11 +2128,11 @@
       <c r="B12" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="57"/>
-      <c r="D12" s="56">
+      <c r="C12" s="56"/>
+      <c r="D12" s="54">
         <v>44004</v>
       </c>
-      <c r="E12" s="56">
+      <c r="E12" s="54">
         <v>44008</v>
       </c>
       <c r="F12" s="12">
@@ -2119,9 +2149,9 @@
       <c r="B13" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="55"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="56"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
       <c r="F13" s="12">
         <v>0</v>
       </c>
@@ -2136,13 +2166,13 @@
       <c r="B14" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="54">
+      <c r="C14" s="55">
         <v>6</v>
       </c>
-      <c r="D14" s="56">
+      <c r="D14" s="54">
         <v>44011</v>
       </c>
-      <c r="E14" s="56">
+      <c r="E14" s="54">
         <v>44016</v>
       </c>
       <c r="F14" s="12">
@@ -2159,9 +2189,9 @@
       <c r="B15" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="55"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
       <c r="F15" s="12">
         <v>0</v>
       </c>
@@ -2176,7 +2206,7 @@
       <c r="B16" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="54">
+      <c r="C16" s="55">
         <v>5</v>
       </c>
       <c r="D16" s="28">
@@ -2199,7 +2229,7 @@
       <c r="B17" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="55"/>
+      <c r="C17" s="57"/>
       <c r="D17" s="28">
         <v>44025</v>
       </c>
@@ -2223,39 +2253,39 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="29"/>
-      <c r="C20" s="50" t="s">
+      <c r="C20" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="50" t="s">
+      <c r="D20" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="50"/>
-      <c r="F20" s="51">
+      <c r="E20" s="40"/>
+      <c r="F20" s="41">
         <f>SUM(F6:F17)/12</f>
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="29"/>
-      <c r="C21" s="50"/>
+      <c r="C21" s="40"/>
       <c r="D21" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="51"/>
+      <c r="F21" s="41"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
-      <c r="C22" s="50"/>
+      <c r="C22" s="40"/>
       <c r="D22" s="4">
         <v>43990</v>
       </c>
       <c r="E22" s="28">
         <v>44029</v>
       </c>
-      <c r="F22" s="51"/>
+      <c r="F22" s="41"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="29"/>
@@ -2265,6 +2295,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="D14:D15"/>
@@ -2279,11 +2314,6 @@
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
   </mergeCells>
   <phoneticPr fontId="31" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
se agregó la página del dashboard, diseño
</commit_message>
<xml_diff>
--- a/Requerimientos/cronograma - AMPLIACIÓN DEL SISTEMA DATA MEDIC.xlsx
+++ b/Requerimientos/cronograma - AMPLIACIÓN DEL SISTEMA DATA MEDIC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DataMedic\Requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01CB179E-D8FF-4AE0-AB5F-722ADE37EF7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6F9D06-CF2B-4DA6-9165-29B0BF064F24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1009,7 +1009,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1103,17 +1103,11 @@
     <xf numFmtId="0" fontId="26" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="25" fillId="28" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="28" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="14" fontId="36" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="30" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1133,22 +1127,22 @@
     <xf numFmtId="14" fontId="36" fillId="26" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="25" fillId="26" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="26" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="26" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="26" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="25" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1166,6 +1160,12 @@
     <xf numFmtId="9" fontId="26" fillId="27" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="25" fillId="28" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="28" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1178,11 +1178,23 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="36" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1509,8 +1521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1524,32 +1536,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="40"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
@@ -1592,14 +1604,14 @@
       <c r="C6" s="32">
         <v>1</v>
       </c>
-      <c r="D6" s="35">
+      <c r="D6" s="54">
         <v>43990</v>
       </c>
-      <c r="E6" s="36"/>
+      <c r="E6" s="55"/>
       <c r="F6" s="33">
         <v>1</v>
       </c>
-      <c r="G6" s="39" t="s">
+      <c r="G6" s="37" t="s">
         <v>17</v>
       </c>
       <c r="H6" s="24"/>
@@ -1615,16 +1627,16 @@
       <c r="C7" s="32">
         <v>2</v>
       </c>
-      <c r="D7" s="61">
+      <c r="D7" s="36">
         <v>43991</v>
       </c>
-      <c r="E7" s="61">
+      <c r="E7" s="36">
         <v>43992</v>
       </c>
       <c r="F7" s="33">
         <v>1</v>
       </c>
-      <c r="G7" s="39"/>
+      <c r="G7" s="37"/>
     </row>
     <row r="8" spans="1:10" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
@@ -1636,14 +1648,14 @@
       <c r="C8" s="32">
         <v>1</v>
       </c>
-      <c r="D8" s="41">
+      <c r="D8" s="39">
         <v>43993</v>
       </c>
-      <c r="E8" s="42"/>
+      <c r="E8" s="40"/>
       <c r="F8" s="33">
         <v>1</v>
       </c>
-      <c r="G8" s="39"/>
+      <c r="G8" s="37"/>
       <c r="H8" s="15"/>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1656,16 +1668,16 @@
       <c r="C9" s="34">
         <v>2</v>
       </c>
-      <c r="D9" s="60">
+      <c r="D9" s="35">
         <v>44000</v>
       </c>
-      <c r="E9" s="60">
+      <c r="E9" s="35">
         <v>44001</v>
       </c>
       <c r="F9" s="33">
         <v>1</v>
       </c>
-      <c r="G9" s="39"/>
+      <c r="G9" s="37"/>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="18">
@@ -1677,14 +1689,14 @@
       <c r="C10" s="34">
         <v>1</v>
       </c>
-      <c r="D10" s="43">
+      <c r="D10" s="41">
         <v>44001</v>
       </c>
-      <c r="E10" s="44"/>
+      <c r="E10" s="42"/>
       <c r="F10" s="33">
         <v>1</v>
       </c>
-      <c r="G10" s="39"/>
+      <c r="G10" s="37"/>
       <c r="H10" s="24"/>
       <c r="I10" s="24"/>
       <c r="J10" s="24"/>
@@ -1693,20 +1705,20 @@
       <c r="A11" s="7">
         <v>6</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="49">
+      <c r="C11" s="47">
         <v>1</v>
       </c>
-      <c r="D11" s="45">
+      <c r="D11" s="43">
         <v>44002</v>
       </c>
-      <c r="E11" s="46"/>
-      <c r="F11" s="11">
+      <c r="E11" s="44"/>
+      <c r="F11" s="33">
         <v>1</v>
       </c>
-      <c r="G11" s="39"/>
+      <c r="G11" s="37"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
@@ -1715,16 +1727,16 @@
       <c r="A12" s="7">
         <v>7</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="50"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="11">
+      <c r="C12" s="48"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="33">
         <v>1</v>
       </c>
-      <c r="G12" s="39"/>
+      <c r="G12" s="37"/>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
@@ -1734,18 +1746,18 @@
         <v>38</v>
       </c>
       <c r="C13" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D13" s="17">
         <v>44004</v>
       </c>
       <c r="E13" s="17">
-        <v>44005</v>
+        <v>44006</v>
       </c>
       <c r="F13" s="11">
         <v>0</v>
       </c>
-      <c r="G13" s="39"/>
+      <c r="G13" s="37"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -1758,15 +1770,15 @@
         <v>2</v>
       </c>
       <c r="D14" s="17">
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="E14" s="17">
-        <v>44007</v>
+        <v>44008</v>
       </c>
       <c r="F14" s="11">
         <v>0</v>
       </c>
-      <c r="G14" s="39"/>
+      <c r="G14" s="37"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
@@ -1775,17 +1787,17 @@
       <c r="B15" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="60">
         <v>1</v>
       </c>
-      <c r="D15" s="37">
-        <v>44008</v>
-      </c>
-      <c r="E15" s="38"/>
+      <c r="D15" s="62">
+        <v>44009</v>
+      </c>
+      <c r="E15" s="63"/>
       <c r="F15" s="11">
         <v>0</v>
       </c>
-      <c r="G15" s="39"/>
+      <c r="G15" s="37"/>
     </row>
     <row r="16" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
@@ -1794,17 +1806,13 @@
       <c r="B16" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="8">
-        <v>1</v>
-      </c>
-      <c r="D16" s="37">
-        <v>44009</v>
-      </c>
-      <c r="E16" s="38"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="65"/>
       <c r="F16" s="11">
         <v>0</v>
       </c>
-      <c r="G16" s="39"/>
+      <c r="G16" s="37"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
@@ -1814,10 +1822,10 @@
         <v>12</v>
       </c>
       <c r="C17" s="12"/>
-      <c r="D17" s="51">
+      <c r="D17" s="49">
         <v>44011</v>
       </c>
-      <c r="E17" s="52"/>
+      <c r="E17" s="50"/>
       <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1831,39 +1839,39 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
-      <c r="C20" s="54" t="s">
+      <c r="C20" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="53" t="s">
+      <c r="D20" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="53"/>
-      <c r="F20" s="55">
+      <c r="E20" s="51"/>
+      <c r="F20" s="53">
         <f>SUM(F6:F16)/11</f>
         <v>0.63636363636363635</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
-      <c r="C21" s="54"/>
+      <c r="C21" s="52"/>
       <c r="D21" s="16" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="55"/>
+      <c r="F21" s="53"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
-      <c r="C22" s="54"/>
+      <c r="C22" s="52"/>
       <c r="D22" s="3">
         <v>43990</v>
       </c>
       <c r="E22" s="3">
         <v>44006</v>
       </c>
-      <c r="F22" s="55"/>
+      <c r="F22" s="53"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="9"/>
@@ -1878,12 +1886,12 @@
     <mergeCell ref="C20:C22"/>
     <mergeCell ref="F20:F22"/>
     <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:E16"/>
     <mergeCell ref="G6:G16"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:F3"/>
-    <mergeCell ref="D15:E15"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D11:E12"/>
@@ -1915,32 +1923,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="40"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -2217,39 +2225,39 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="27"/>
-      <c r="C20" s="54" t="s">
+      <c r="C20" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="54" t="s">
+      <c r="D20" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="54"/>
-      <c r="F20" s="55">
+      <c r="E20" s="52"/>
+      <c r="F20" s="53">
         <f>SUM(F6:F17)/12</f>
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="27"/>
-      <c r="C21" s="54"/>
+      <c r="C21" s="52"/>
       <c r="D21" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="55"/>
+      <c r="F21" s="53"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
-      <c r="C22" s="54"/>
+      <c r="C22" s="52"/>
       <c r="D22" s="3">
         <v>43990</v>
       </c>
       <c r="E22" s="26">
         <v>44029</v>
       </c>
-      <c r="F22" s="55"/>
+      <c r="F22" s="53"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="27"/>

</xml_diff>

<commit_message>
se arregló el problema de registrar horario_atencion y se agregó el reporte 1, pero falta cita denegada
</commit_message>
<xml_diff>
--- a/Requerimientos/cronograma - AMPLIACIÓN DEL SISTEMA DATA MEDIC.xlsx
+++ b/Requerimientos/cronograma - AMPLIACIÓN DEL SISTEMA DATA MEDIC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DataMedic\Requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6F9D06-CF2B-4DA6-9165-29B0BF064F24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0A5198-8BEE-42C2-896D-DBB527A30C80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1109,6 +1109,45 @@
     <xf numFmtId="14" fontId="25" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="25" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="26" fillId="27" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="28" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="28" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="30" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1145,55 +1184,16 @@
     <xf numFmtId="0" fontId="1" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="25" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="26" fillId="27" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="28" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="28" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1522,7 +1522,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D17" sqref="D17:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1536,32 +1536,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
+      <c r="A3" s="51"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
@@ -1604,14 +1604,14 @@
       <c r="C6" s="32">
         <v>1</v>
       </c>
-      <c r="D6" s="54">
+      <c r="D6" s="42">
         <v>43990</v>
       </c>
-      <c r="E6" s="55"/>
+      <c r="E6" s="43"/>
       <c r="F6" s="33">
         <v>1</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="G6" s="50" t="s">
         <v>17</v>
       </c>
       <c r="H6" s="24"/>
@@ -1636,7 +1636,7 @@
       <c r="F7" s="33">
         <v>1</v>
       </c>
-      <c r="G7" s="37"/>
+      <c r="G7" s="50"/>
     </row>
     <row r="8" spans="1:10" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
@@ -1648,14 +1648,14 @@
       <c r="C8" s="32">
         <v>1</v>
       </c>
-      <c r="D8" s="39">
+      <c r="D8" s="52">
         <v>43993</v>
       </c>
-      <c r="E8" s="40"/>
+      <c r="E8" s="53"/>
       <c r="F8" s="33">
         <v>1</v>
       </c>
-      <c r="G8" s="37"/>
+      <c r="G8" s="50"/>
       <c r="H8" s="15"/>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1677,7 +1677,7 @@
       <c r="F9" s="33">
         <v>1</v>
       </c>
-      <c r="G9" s="37"/>
+      <c r="G9" s="50"/>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="18">
@@ -1689,14 +1689,14 @@
       <c r="C10" s="34">
         <v>1</v>
       </c>
-      <c r="D10" s="41">
+      <c r="D10" s="54">
         <v>44001</v>
       </c>
-      <c r="E10" s="42"/>
+      <c r="E10" s="55"/>
       <c r="F10" s="33">
         <v>1</v>
       </c>
-      <c r="G10" s="37"/>
+      <c r="G10" s="50"/>
       <c r="H10" s="24"/>
       <c r="I10" s="24"/>
       <c r="J10" s="24"/>
@@ -1708,17 +1708,17 @@
       <c r="B11" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="47">
+      <c r="C11" s="60">
         <v>1</v>
       </c>
-      <c r="D11" s="43">
+      <c r="D11" s="56">
         <v>44002</v>
       </c>
-      <c r="E11" s="44"/>
+      <c r="E11" s="57"/>
       <c r="F11" s="33">
         <v>1</v>
       </c>
-      <c r="G11" s="37"/>
+      <c r="G11" s="50"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
@@ -1730,13 +1730,13 @@
       <c r="B12" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="46"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="59"/>
       <c r="F12" s="33">
         <v>1</v>
       </c>
-      <c r="G12" s="37"/>
+      <c r="G12" s="50"/>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
@@ -1749,15 +1749,15 @@
         <v>3</v>
       </c>
       <c r="D13" s="17">
-        <v>44004</v>
+        <v>44006</v>
       </c>
       <c r="E13" s="17">
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="F13" s="11">
         <v>0</v>
       </c>
-      <c r="G13" s="37"/>
+      <c r="G13" s="50"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -1770,34 +1770,34 @@
         <v>2</v>
       </c>
       <c r="D14" s="17">
-        <v>44007</v>
+        <v>44008</v>
       </c>
       <c r="E14" s="17">
-        <v>44008</v>
+        <v>44009</v>
       </c>
       <c r="F14" s="11">
         <v>0</v>
       </c>
-      <c r="G14" s="37"/>
+      <c r="G14" s="50"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>10</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="60">
+      <c r="C15" s="44">
         <v>1</v>
       </c>
-      <c r="D15" s="62">
+      <c r="D15" s="46">
         <v>44009</v>
       </c>
-      <c r="E15" s="63"/>
+      <c r="E15" s="47"/>
       <c r="F15" s="11">
-        <v>0</v>
-      </c>
-      <c r="G15" s="37"/>
+        <v>1</v>
+      </c>
+      <c r="G15" s="50"/>
     </row>
     <row r="16" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
@@ -1806,13 +1806,13 @@
       <c r="B16" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="61"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="65"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="49"/>
       <c r="F16" s="11">
         <v>0</v>
       </c>
-      <c r="G16" s="37"/>
+      <c r="G16" s="50"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
@@ -1822,10 +1822,10 @@
         <v>12</v>
       </c>
       <c r="C17" s="12"/>
-      <c r="D17" s="49">
+      <c r="D17" s="37">
         <v>44011</v>
       </c>
-      <c r="E17" s="50"/>
+      <c r="E17" s="38"/>
       <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1839,39 +1839,39 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
-      <c r="C20" s="52" t="s">
+      <c r="C20" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="51" t="s">
+      <c r="D20" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="51"/>
-      <c r="F20" s="53">
+      <c r="E20" s="39"/>
+      <c r="F20" s="41">
         <f>SUM(F6:F16)/11</f>
-        <v>0.63636363636363635</v>
+        <v>0.72727272727272729</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
-      <c r="C21" s="52"/>
+      <c r="C21" s="40"/>
       <c r="D21" s="16" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="53"/>
+      <c r="F21" s="41"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
-      <c r="C22" s="52"/>
+      <c r="C22" s="40"/>
       <c r="D22" s="3">
         <v>43990</v>
       </c>
       <c r="E22" s="3">
         <v>44006</v>
       </c>
-      <c r="F22" s="53"/>
+      <c r="F22" s="41"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="9"/>
@@ -1881,13 +1881,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:E16"/>
     <mergeCell ref="G6:G16"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A1:F1"/>
@@ -1896,6 +1889,13 @@
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D11:E12"/>
     <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1923,32 +1923,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
+      <c r="A3" s="51"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -1980,13 +1980,13 @@
       <c r="B6" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="56">
+      <c r="C6" s="63">
         <v>5</v>
       </c>
-      <c r="D6" s="58">
+      <c r="D6" s="62">
         <v>43990</v>
       </c>
-      <c r="E6" s="58">
+      <c r="E6" s="62">
         <v>43994</v>
       </c>
       <c r="F6" s="11">
@@ -2003,9 +2003,9 @@
       <c r="B7" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="59"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
       <c r="F7" s="11">
         <v>0</v>
       </c>
@@ -2020,11 +2020,11 @@
       <c r="B8" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="59"/>
-      <c r="D8" s="58">
+      <c r="C8" s="64"/>
+      <c r="D8" s="62">
         <v>43997</v>
       </c>
-      <c r="E8" s="58">
+      <c r="E8" s="62">
         <v>44001</v>
       </c>
       <c r="F8" s="11">
@@ -2042,9 +2042,9 @@
       <c r="B9" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="59"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62"/>
       <c r="F9" s="11">
         <v>0</v>
       </c>
@@ -2059,11 +2059,11 @@
       <c r="B10" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="59"/>
-      <c r="D10" s="58">
+      <c r="C10" s="64"/>
+      <c r="D10" s="62">
         <v>44004</v>
       </c>
-      <c r="E10" s="58">
+      <c r="E10" s="62">
         <v>44008</v>
       </c>
       <c r="F10" s="11">
@@ -2080,9 +2080,9 @@
       <c r="B11" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="59"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
       <c r="F11" s="11">
         <v>0</v>
       </c>
@@ -2100,11 +2100,11 @@
       <c r="B12" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="59"/>
-      <c r="D12" s="58">
+      <c r="C12" s="64"/>
+      <c r="D12" s="62">
         <v>44004</v>
       </c>
-      <c r="E12" s="58">
+      <c r="E12" s="62">
         <v>44008</v>
       </c>
       <c r="F12" s="11">
@@ -2121,9 +2121,9 @@
       <c r="B13" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="57"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="58"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
       <c r="F13" s="11">
         <v>0</v>
       </c>
@@ -2138,13 +2138,13 @@
       <c r="B14" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="56">
+      <c r="C14" s="63">
         <v>6</v>
       </c>
-      <c r="D14" s="58">
+      <c r="D14" s="62">
         <v>44011</v>
       </c>
-      <c r="E14" s="58">
+      <c r="E14" s="62">
         <v>44016</v>
       </c>
       <c r="F14" s="11">
@@ -2161,9 +2161,9 @@
       <c r="B15" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="57"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="58"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="62"/>
       <c r="F15" s="11">
         <v>0</v>
       </c>
@@ -2178,7 +2178,7 @@
       <c r="B16" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="56">
+      <c r="C16" s="63">
         <v>5</v>
       </c>
       <c r="D16" s="26">
@@ -2201,7 +2201,7 @@
       <c r="B17" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="57"/>
+      <c r="C17" s="65"/>
       <c r="D17" s="26">
         <v>44025</v>
       </c>
@@ -2225,39 +2225,39 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="27"/>
-      <c r="C20" s="52" t="s">
+      <c r="C20" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="52" t="s">
+      <c r="D20" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="52"/>
-      <c r="F20" s="53">
+      <c r="E20" s="40"/>
+      <c r="F20" s="41">
         <f>SUM(F6:F17)/12</f>
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="27"/>
-      <c r="C21" s="52"/>
+      <c r="C21" s="40"/>
       <c r="D21" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="53"/>
+      <c r="F21" s="41"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
-      <c r="C22" s="52"/>
+      <c r="C22" s="40"/>
       <c r="D22" s="3">
         <v>43990</v>
       </c>
       <c r="E22" s="26">
         <v>44029</v>
       </c>
-      <c r="F22" s="53"/>
+      <c r="F22" s="41"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="27"/>
@@ -2267,6 +2267,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="D14:D15"/>
@@ -2281,11 +2286,6 @@
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
   </mergeCells>
   <phoneticPr fontId="30" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
se terminó de hacer el dashboar
</commit_message>
<xml_diff>
--- a/Requerimientos/cronograma - AMPLIACIÓN DEL SISTEMA DATA MEDIC.xlsx
+++ b/Requerimientos/cronograma - AMPLIACIÓN DEL SISTEMA DATA MEDIC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DataMedic\Requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0A5198-8BEE-42C2-896D-DBB527A30C80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5752F84C-969D-42DF-A19E-2D8179168A07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1109,6 +1109,42 @@
     <xf numFmtId="14" fontId="25" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="30" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="26" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="26" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="36" fillId="26" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="36" fillId="26" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="26" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="26" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="26" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="26" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="25" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1148,52 +1184,16 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="30" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="26" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="26" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="36" fillId="26" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="36" fillId="26" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="26" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="26" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="26" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="26" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1536,32 +1536,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="51"/>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
@@ -1604,14 +1604,14 @@
       <c r="C6" s="32">
         <v>1</v>
       </c>
-      <c r="D6" s="42">
+      <c r="D6" s="54">
         <v>43990</v>
       </c>
-      <c r="E6" s="43"/>
+      <c r="E6" s="55"/>
       <c r="F6" s="33">
         <v>1</v>
       </c>
-      <c r="G6" s="50" t="s">
+      <c r="G6" s="37" t="s">
         <v>17</v>
       </c>
       <c r="H6" s="24"/>
@@ -1636,7 +1636,7 @@
       <c r="F7" s="33">
         <v>1</v>
       </c>
-      <c r="G7" s="50"/>
+      <c r="G7" s="37"/>
     </row>
     <row r="8" spans="1:10" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
@@ -1648,14 +1648,14 @@
       <c r="C8" s="32">
         <v>1</v>
       </c>
-      <c r="D8" s="52">
+      <c r="D8" s="39">
         <v>43993</v>
       </c>
-      <c r="E8" s="53"/>
+      <c r="E8" s="40"/>
       <c r="F8" s="33">
         <v>1</v>
       </c>
-      <c r="G8" s="50"/>
+      <c r="G8" s="37"/>
       <c r="H8" s="15"/>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1677,7 +1677,7 @@
       <c r="F9" s="33">
         <v>1</v>
       </c>
-      <c r="G9" s="50"/>
+      <c r="G9" s="37"/>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="18">
@@ -1689,14 +1689,14 @@
       <c r="C10" s="34">
         <v>1</v>
       </c>
-      <c r="D10" s="54">
+      <c r="D10" s="41">
         <v>44001</v>
       </c>
-      <c r="E10" s="55"/>
+      <c r="E10" s="42"/>
       <c r="F10" s="33">
         <v>1</v>
       </c>
-      <c r="G10" s="50"/>
+      <c r="G10" s="37"/>
       <c r="H10" s="24"/>
       <c r="I10" s="24"/>
       <c r="J10" s="24"/>
@@ -1708,17 +1708,17 @@
       <c r="B11" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="60">
+      <c r="C11" s="47">
         <v>1</v>
       </c>
-      <c r="D11" s="56">
+      <c r="D11" s="43">
         <v>44002</v>
       </c>
-      <c r="E11" s="57"/>
+      <c r="E11" s="44"/>
       <c r="F11" s="33">
         <v>1</v>
       </c>
-      <c r="G11" s="50"/>
+      <c r="G11" s="37"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
@@ -1730,13 +1730,13 @@
       <c r="B12" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="61"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="59"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="33">
         <v>1</v>
       </c>
-      <c r="G12" s="50"/>
+      <c r="G12" s="37"/>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
@@ -1757,7 +1757,7 @@
       <c r="F13" s="11">
         <v>0</v>
       </c>
-      <c r="G13" s="50"/>
+      <c r="G13" s="37"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -1778,7 +1778,7 @@
       <c r="F14" s="11">
         <v>0</v>
       </c>
-      <c r="G14" s="50"/>
+      <c r="G14" s="37"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
@@ -1787,17 +1787,17 @@
       <c r="B15" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="44">
+      <c r="C15" s="56">
         <v>1</v>
       </c>
-      <c r="D15" s="46">
+      <c r="D15" s="58">
         <v>44009</v>
       </c>
-      <c r="E15" s="47"/>
+      <c r="E15" s="59"/>
       <c r="F15" s="11">
         <v>1</v>
       </c>
-      <c r="G15" s="50"/>
+      <c r="G15" s="37"/>
     </row>
     <row r="16" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
@@ -1806,13 +1806,13 @@
       <c r="B16" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="45"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="49"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="61"/>
       <c r="F16" s="11">
         <v>0</v>
       </c>
-      <c r="G16" s="50"/>
+      <c r="G16" s="37"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
@@ -1822,10 +1822,10 @@
         <v>12</v>
       </c>
       <c r="C17" s="12"/>
-      <c r="D17" s="37">
+      <c r="D17" s="49">
         <v>44011</v>
       </c>
-      <c r="E17" s="38"/>
+      <c r="E17" s="50"/>
       <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1839,39 +1839,39 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
-      <c r="C20" s="40" t="s">
+      <c r="C20" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="39" t="s">
+      <c r="D20" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="39"/>
-      <c r="F20" s="41">
+      <c r="E20" s="51"/>
+      <c r="F20" s="53">
         <f>SUM(F6:F16)/11</f>
         <v>0.72727272727272729</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
-      <c r="C21" s="40"/>
+      <c r="C21" s="52"/>
       <c r="D21" s="16" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="41"/>
+      <c r="F21" s="53"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
-      <c r="C22" s="40"/>
+      <c r="C22" s="52"/>
       <c r="D22" s="3">
         <v>43990</v>
       </c>
       <c r="E22" s="3">
         <v>44006</v>
       </c>
-      <c r="F22" s="41"/>
+      <c r="F22" s="53"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="9"/>
@@ -1881,6 +1881,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:E16"/>
     <mergeCell ref="G6:G16"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A1:F1"/>
@@ -1889,13 +1896,6 @@
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D11:E12"/>
     <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1923,32 +1923,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="51"/>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -1980,13 +1980,13 @@
       <c r="B6" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="63">
+      <c r="C6" s="62">
         <v>5</v>
       </c>
-      <c r="D6" s="62">
+      <c r="D6" s="64">
         <v>43990</v>
       </c>
-      <c r="E6" s="62">
+      <c r="E6" s="64">
         <v>43994</v>
       </c>
       <c r="F6" s="11">
@@ -2003,9 +2003,9 @@
       <c r="B7" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="64"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
       <c r="F7" s="11">
         <v>0</v>
       </c>
@@ -2020,11 +2020,11 @@
       <c r="B8" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="64"/>
-      <c r="D8" s="62">
+      <c r="C8" s="65"/>
+      <c r="D8" s="64">
         <v>43997</v>
       </c>
-      <c r="E8" s="62">
+      <c r="E8" s="64">
         <v>44001</v>
       </c>
       <c r="F8" s="11">
@@ -2042,9 +2042,9 @@
       <c r="B9" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="64"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
       <c r="F9" s="11">
         <v>0</v>
       </c>
@@ -2059,11 +2059,11 @@
       <c r="B10" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="64"/>
-      <c r="D10" s="62">
+      <c r="C10" s="65"/>
+      <c r="D10" s="64">
         <v>44004</v>
       </c>
-      <c r="E10" s="62">
+      <c r="E10" s="64">
         <v>44008</v>
       </c>
       <c r="F10" s="11">
@@ -2080,9 +2080,9 @@
       <c r="B11" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="64"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="62"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
       <c r="F11" s="11">
         <v>0</v>
       </c>
@@ -2100,11 +2100,11 @@
       <c r="B12" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="64"/>
-      <c r="D12" s="62">
+      <c r="C12" s="65"/>
+      <c r="D12" s="64">
         <v>44004</v>
       </c>
-      <c r="E12" s="62">
+      <c r="E12" s="64">
         <v>44008</v>
       </c>
       <c r="F12" s="11">
@@ -2121,9 +2121,9 @@
       <c r="B13" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="65"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
       <c r="F13" s="11">
         <v>0</v>
       </c>
@@ -2138,13 +2138,13 @@
       <c r="B14" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="63">
+      <c r="C14" s="62">
         <v>6</v>
       </c>
-      <c r="D14" s="62">
+      <c r="D14" s="64">
         <v>44011</v>
       </c>
-      <c r="E14" s="62">
+      <c r="E14" s="64">
         <v>44016</v>
       </c>
       <c r="F14" s="11">
@@ -2161,9 +2161,9 @@
       <c r="B15" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="65"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
       <c r="F15" s="11">
         <v>0</v>
       </c>
@@ -2178,7 +2178,7 @@
       <c r="B16" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="63">
+      <c r="C16" s="62">
         <v>5</v>
       </c>
       <c r="D16" s="26">
@@ -2201,7 +2201,7 @@
       <c r="B17" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="65"/>
+      <c r="C17" s="63"/>
       <c r="D17" s="26">
         <v>44025</v>
       </c>
@@ -2225,39 +2225,39 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="27"/>
-      <c r="C20" s="40" t="s">
+      <c r="C20" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="40" t="s">
+      <c r="D20" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="40"/>
-      <c r="F20" s="41">
+      <c r="E20" s="52"/>
+      <c r="F20" s="53">
         <f>SUM(F6:F17)/12</f>
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="27"/>
-      <c r="C21" s="40"/>
+      <c r="C21" s="52"/>
       <c r="D21" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="41"/>
+      <c r="F21" s="53"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
-      <c r="C22" s="40"/>
+      <c r="C22" s="52"/>
       <c r="D22" s="3">
         <v>43990</v>
       </c>
       <c r="E22" s="26">
         <v>44029</v>
       </c>
-      <c r="F22" s="41"/>
+      <c r="F22" s="53"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="27"/>
@@ -2267,11 +2267,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="D14:D15"/>
@@ -2286,6 +2281,11 @@
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
   </mergeCells>
   <phoneticPr fontId="30" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>